<commit_message>
econ: harvest and haul costs from cubic volume
</commit_message>
<xml_diff>
--- a/UnitTests/financial scenarios.xlsx
+++ b/UnitTests/financial scenarios.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>name</t>
   </si>
@@ -38,30 +38,15 @@
     <t>sitePrepFixed</t>
   </si>
   <si>
-    <t>regenFixed</t>
-  </si>
-  <si>
     <t>releaseSpray</t>
   </si>
   <si>
-    <t>thinFixed</t>
-  </si>
-  <si>
     <t>seedling</t>
   </si>
   <si>
-    <t>annualTaxAndManagement</t>
-  </si>
-  <si>
     <t>timberAppreciation</t>
   </si>
   <si>
-    <t>regenPerMbf</t>
-  </si>
-  <si>
-    <t>thinPerMbf</t>
-  </si>
-  <si>
     <t>psme2Spond</t>
   </si>
   <si>
@@ -81,6 +66,33 @@
   </si>
   <si>
     <t>white4Spond</t>
+  </si>
+  <si>
+    <t>thinPondMultiplier</t>
+  </si>
+  <si>
+    <t>thinPerHa</t>
+  </si>
+  <si>
+    <t>regenPerHa</t>
+  </si>
+  <si>
+    <t>regenHarvestPerM3</t>
+  </si>
+  <si>
+    <t>regenHaulPerM3</t>
+  </si>
+  <si>
+    <t>thinHarvestPerM3</t>
+  </si>
+  <si>
+    <t>thinHaulPerM3</t>
+  </si>
+  <si>
+    <t>harvestTaxPerMbf</t>
+  </si>
+  <si>
+    <t>propertyTaxAndManagementPerHa</t>
   </si>
 </sst>
 </file>
@@ -399,23 +411,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="11" max="11" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.33203125" customWidth="1"/>
-    <col min="15" max="15" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5546875" customWidth="1"/>
+    <col min="15" max="15" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.33203125" customWidth="1"/>
+    <col min="17" max="17" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -423,55 +436,67 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>3</v>
+      </c>
+      <c r="R1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" t="s">
-        <v>7</v>
-      </c>
-      <c r="O1" t="s">
-        <v>3</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="V1" t="s">
         <v>6</v>
       </c>
-      <c r="Q1" t="s">
-        <v>11</v>
-      </c>
-      <c r="R1" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -502,29 +527,41 @@
       <c r="J2">
         <v>18.53</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K2">
+        <v>4.1322000000000001</v>
+      </c>
+      <c r="L2" s="1">
         <v>247</v>
       </c>
-      <c r="L2" s="1">
-        <v>250</v>
-      </c>
       <c r="M2" s="1">
+        <v>17</v>
+      </c>
+      <c r="N2" s="1">
+        <v>8.51</v>
+      </c>
+      <c r="O2" s="1">
         <v>74.099999999999994</v>
       </c>
-      <c r="N2" s="1">
+      <c r="P2" s="1">
         <v>0.5</v>
       </c>
-      <c r="O2" s="1">
+      <c r="Q2" s="1">
         <f>2.47*(136+154)</f>
         <v>716.30000000000007</v>
       </c>
-      <c r="P2" s="1">
+      <c r="R2" s="1">
         <v>148.19999999999999</v>
       </c>
-      <c r="Q2" s="1">
-        <v>275</v>
-      </c>
-      <c r="R2" s="1">
+      <c r="S2" s="1">
+        <v>19.5</v>
+      </c>
+      <c r="T2" s="1">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="U2" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="V2" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
econ: include machine productivity in harvest cost
</commit_message>
<xml_diff>
--- a/UnitTests/financial scenarios.xlsx
+++ b/UnitTests/financial scenarios.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>name</t>
   </si>
@@ -77,15 +77,9 @@
     <t>regenPerHa</t>
   </si>
   <si>
-    <t>regenHarvestPerM3</t>
-  </si>
-  <si>
     <t>regenHaulPerM3</t>
   </si>
   <si>
-    <t>thinHarvestPerM3</t>
-  </si>
-  <si>
     <t>thinHaulPerM3</t>
   </si>
   <si>
@@ -93,14 +87,127 @@
   </si>
   <si>
     <t>propertyTaxAndManagementPerHa</t>
+  </si>
+  <si>
+    <t>corridorWidth</t>
+  </si>
+  <si>
+    <t>forwarderPayload</t>
+  </si>
+  <si>
+    <t>forwarderLoadedTethered</t>
+  </si>
+  <si>
+    <t>forwarderLoadedUntethered</t>
+  </si>
+  <si>
+    <t>forwarderUnloadedTethered</t>
+  </si>
+  <si>
+    <t>forwarderOnRoad</t>
+  </si>
+  <si>
+    <t>harvesterConstant</t>
+  </si>
+  <si>
+    <t>harvesterLinear</t>
+  </si>
+  <si>
+    <t>harvesterQuadratic</t>
+  </si>
+  <si>
+    <t>harvesterQuadraticThreshold</t>
+  </si>
+  <si>
+    <t>harvesterSlopeThreshold</t>
+  </si>
+  <si>
+    <t>forwarderUnloadedUntethered</t>
+  </si>
+  <si>
+    <t>fellerBuncherConstant</t>
+  </si>
+  <si>
+    <t>fellerBuncherLinear</t>
+  </si>
+  <si>
+    <t>fellerBuncherSlopeThreshold</t>
+  </si>
+  <si>
+    <t>processorConstant</t>
+  </si>
+  <si>
+    <t>processorLinear</t>
+  </si>
+  <si>
+    <t>processorQuadratic1</t>
+  </si>
+  <si>
+    <t>processorQuadraticThreshold1</t>
+  </si>
+  <si>
+    <t>processorQuadratic2</t>
+  </si>
+  <si>
+    <t>processorQuadraticThreshold2</t>
+  </si>
+  <si>
+    <t>loaderProductivity</t>
+  </si>
+  <si>
+    <t>grappleYardingConstant</t>
+  </si>
+  <si>
+    <t>grappleYardingLinear</t>
+  </si>
+  <si>
+    <t>grappleYoaderMeanPayload</t>
+  </si>
+  <si>
+    <t>grappleYoaderUtilization</t>
+  </si>
+  <si>
+    <t>processorUtilization</t>
+  </si>
+  <si>
+    <t>loaderUtilization</t>
+  </si>
+  <si>
+    <t>loaderSMh</t>
+  </si>
+  <si>
+    <t>processorSMh</t>
+  </si>
+  <si>
+    <t>grappleYoaderSMh</t>
+  </si>
+  <si>
+    <t>forwarderPMh</t>
+  </si>
+  <si>
+    <t>harvesterPMh</t>
+  </si>
+  <si>
+    <t>fellerBuncherPMh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -128,9 +235,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,92 +521,190 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:BB2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="12" max="12" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.5546875" customWidth="1"/>
+    <col min="14" max="14" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.33203125" customWidth="1"/>
     <col min="17" max="17" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="30" width="11.77734375" customWidth="1"/>
+    <col min="31" max="31" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="S1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AO1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AP1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AR1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AS1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AT1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AU1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AV1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AW1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AX1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AY1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AZ1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="BA1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="BB1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N1" t="s">
-        <v>18</v>
-      </c>
-      <c r="O1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P1" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>3</v>
-      </c>
-      <c r="R1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T1" t="s">
-        <v>20</v>
-      </c>
-      <c r="U1" t="s">
-        <v>14</v>
-      </c>
-      <c r="V1" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -504,68 +712,167 @@
         <v>0.04</v>
       </c>
       <c r="C2">
-        <v>611</v>
+        <v>649</v>
       </c>
       <c r="D2">
-        <v>595</v>
+        <v>635</v>
       </c>
       <c r="E2">
-        <v>508</v>
+        <v>552</v>
       </c>
       <c r="F2">
-        <v>1150</v>
+        <v>1238</v>
       </c>
       <c r="G2">
-        <v>497</v>
+        <v>531</v>
       </c>
       <c r="H2">
-        <v>491</v>
+        <v>525</v>
       </c>
       <c r="I2">
-        <v>417</v>
-      </c>
-      <c r="J2">
-        <v>18.53</v>
+        <v>454</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0</v>
       </c>
       <c r="K2">
+        <v>37.71</v>
+      </c>
+      <c r="L2">
         <v>4.1322000000000001</v>
       </c>
-      <c r="L2" s="1">
-        <v>247</v>
-      </c>
-      <c r="M2" s="1">
-        <v>17</v>
+      <c r="M2">
+        <v>15</v>
       </c>
       <c r="N2" s="1">
-        <v>8.51</v>
+        <f>65+32+5*2*(2*10+3*170)/15+25+45</f>
+        <v>520.33333333333326</v>
       </c>
       <c r="O2" s="1">
-        <v>74.099999999999994</v>
+        <v>275</v>
       </c>
       <c r="P2" s="1">
         <v>0.5</v>
       </c>
       <c r="Q2" s="1">
-        <f>2.47*(136+154)</f>
-        <v>716.30000000000007</v>
-      </c>
-      <c r="R2" s="1">
-        <v>148.19999999999999</v>
-      </c>
-      <c r="S2" s="1">
-        <v>19.5</v>
-      </c>
-      <c r="T2" s="1">
+        <f>145+200+383</f>
+        <v>728</v>
+      </c>
+      <c r="R2" s="4">
+        <v>20000</v>
+      </c>
+      <c r="S2" s="4">
+        <v>33</v>
+      </c>
+      <c r="T2" s="4">
+        <v>45</v>
+      </c>
+      <c r="U2" s="4">
+        <v>50</v>
+      </c>
+      <c r="V2" s="4">
+        <v>60</v>
+      </c>
+      <c r="W2" s="4">
+        <v>66</v>
+      </c>
+      <c r="X2" s="1">
+        <v>258</v>
+      </c>
+      <c r="Y2" s="4">
+        <v>28</v>
+      </c>
+      <c r="Z2" s="4">
+        <v>43</v>
+      </c>
+      <c r="AA2" s="4">
+        <v>6</v>
+      </c>
+      <c r="AB2" s="3">
+        <v>1.9</v>
+      </c>
+      <c r="AC2" s="4">
+        <v>45</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>308</v>
+      </c>
+      <c r="AE2" s="1">
+        <f>65+32+3*2*(2*10+3*170)/15+25+45</f>
+        <v>379</v>
+      </c>
+      <c r="AF2" s="1">
         <v>9.8000000000000007</v>
       </c>
-      <c r="U2" s="1">
+      <c r="AG2" s="1">
         <v>0.9</v>
       </c>
-      <c r="V2" s="1">
-        <v>0</v>
+      <c r="AH2" s="4">
+        <v>14</v>
+      </c>
+      <c r="AI2">
+        <v>4.7</v>
+      </c>
+      <c r="AJ2">
+        <v>30</v>
+      </c>
+      <c r="AK2" s="1">
+        <v>274</v>
+      </c>
+      <c r="AL2">
+        <v>45</v>
+      </c>
+      <c r="AM2">
+        <v>0.72</v>
+      </c>
+      <c r="AN2">
+        <v>1550</v>
+      </c>
+      <c r="AO2" s="1">
+        <v>239</v>
+      </c>
+      <c r="AP2">
+        <v>0.75</v>
+      </c>
+      <c r="AQ2">
+        <v>21</v>
+      </c>
+      <c r="AR2">
+        <v>30</v>
+      </c>
+      <c r="AS2">
+        <v>1.5</v>
+      </c>
+      <c r="AT2">
+        <v>2.5</v>
+      </c>
+      <c r="AU2">
+        <v>4.5</v>
+      </c>
+      <c r="AV2" s="3">
+        <v>6</v>
+      </c>
+      <c r="AW2" s="1">
+        <v>179</v>
+      </c>
+      <c r="AX2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="AY2">
+        <v>72.400000000000006</v>
+      </c>
+      <c r="AZ2" s="1">
+        <v>151</v>
+      </c>
+      <c r="BA2">
+        <v>0.85</v>
+      </c>
+      <c r="BB2" s="1">
+        <v>10.17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
econ: include manual bucking in harvest cost of trees too large for mechanized processing
</commit_message>
<xml_diff>
--- a/UnitTests/financial scenarios.xlsx
+++ b/UnitTests/financial scenarios.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21852" windowHeight="7680"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16188" windowHeight="7572"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>name</t>
   </si>
@@ -107,21 +107,6 @@
     <t>forwarderOnRoad</t>
   </si>
   <si>
-    <t>harvesterConstant</t>
-  </si>
-  <si>
-    <t>harvesterLinear</t>
-  </si>
-  <si>
-    <t>harvesterQuadratic</t>
-  </si>
-  <si>
-    <t>harvesterQuadraticThreshold</t>
-  </si>
-  <si>
-    <t>harvesterSlopeThreshold</t>
-  </si>
-  <si>
     <t>forwarderUnloadedUntethered</t>
   </si>
   <si>
@@ -185,20 +170,87 @@
     <t>forwarderPMh</t>
   </si>
   <si>
-    <t>harvesterPMh</t>
-  </si>
-  <si>
     <t>fellerBuncherPMh</t>
+  </si>
+  <si>
+    <t>chainsawProductivity</t>
+  </si>
+  <si>
+    <t>chainsawPMh</t>
+  </si>
+  <si>
+    <t>grappleYoaderMaxPayload</t>
+  </si>
+  <si>
+    <t>grappleSwingYarderMaxPayload</t>
+  </si>
+  <si>
+    <t>grappleSwingYarderMeanPayload</t>
+  </si>
+  <si>
+    <t>grappleSwingYarderSMh</t>
+  </si>
+  <si>
+    <t>grappleSwingYarderUtilization</t>
+  </si>
+  <si>
+    <t>wheeledHarvesterDiameterLimit</t>
+  </si>
+  <si>
+    <t>wheeledHarvesterConstant</t>
+  </si>
+  <si>
+    <t>wheeledHarvesterLinear</t>
+  </si>
+  <si>
+    <t>wheeledHarvesterQuadratic</t>
+  </si>
+  <si>
+    <t>wheeledHarvesterQuadraticThreshold</t>
+  </si>
+  <si>
+    <t>wheeledHarvesterSlopeThreshold</t>
+  </si>
+  <si>
+    <t>wheeledHarvesterPMh</t>
+  </si>
+  <si>
+    <t>trackedHarvesterDiameterLimit</t>
+  </si>
+  <si>
+    <t>trackedHarvesterConstant</t>
+  </si>
+  <si>
+    <t>trackedHarvesterLinear</t>
+  </si>
+  <si>
+    <t>trackedHarvesterSlopeThreshold</t>
+  </si>
+  <si>
+    <t>trackedHarvesterPMh</t>
+  </si>
+  <si>
+    <t>trackedHarvesterQuadraticThreshold1</t>
+  </si>
+  <si>
+    <t>trackedHarvesterQuadraticThreshold2</t>
+  </si>
+  <si>
+    <t>trackedHarvesterQuadratic1</t>
+  </si>
+  <si>
+    <t>trackedHarvesterQuadratic2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,6 +260,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -232,17 +291,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -521,13 +583,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BB2"/>
+  <dimension ref="A1:BS2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -536,11 +598,11 @@
     <col min="15" max="15" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.33203125" customWidth="1"/>
     <col min="17" max="17" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="18" max="30" width="11.77734375" customWidth="1"/>
-    <col min="31" max="31" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="31" width="11.77734375" customWidth="1"/>
+    <col min="32" max="32" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -605,106 +667,157 @@
         <v>25</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="W1" s="2" t="s">
         <v>26</v>
       </c>
       <c r="X1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AO1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AR1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AS1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AT1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AU1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AV1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AW1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AX1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AY1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AZ1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="Y1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC1" s="2" t="s">
+      <c r="BA1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="BB1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="BC1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="BD1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="BE1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="BF1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="BG1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="BH1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AD1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="AH1" s="2" t="s">
+      <c r="BI1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="BJ1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="BK1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="BL1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AL1" s="2" t="s">
+      <c r="BM1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BN1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="BO1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="BP1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="BQ1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="BR1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AM1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AN1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AO1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AP1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AQ1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AR1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AS1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AT1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AU1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="AV1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AW1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AX1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="AY1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AZ1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="BA1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="BB1" s="2" t="s">
+      <c r="BS1" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -780,94 +893,145 @@
         <v>258</v>
       </c>
       <c r="Y2" s="4">
+        <v>70</v>
+      </c>
+      <c r="Z2" s="4">
         <v>28</v>
       </c>
-      <c r="Z2" s="4">
+      <c r="AA2" s="4">
         <v>43</v>
       </c>
-      <c r="AA2" s="4">
+      <c r="AB2" s="4">
         <v>6</v>
       </c>
-      <c r="AB2" s="3">
+      <c r="AC2" s="3">
         <v>1.9</v>
       </c>
-      <c r="AC2" s="4">
+      <c r="AD2" s="4">
         <v>45</v>
       </c>
-      <c r="AD2" s="1">
+      <c r="AE2" s="1">
         <v>308</v>
       </c>
-      <c r="AE2" s="1">
+      <c r="AF2" s="1">
         <f>65+32+3*2*(2*10+3*170)/15+25+45</f>
         <v>379</v>
       </c>
-      <c r="AF2" s="1">
+      <c r="AG2" s="1">
         <v>9.8000000000000007</v>
       </c>
-      <c r="AG2" s="1">
+      <c r="AH2" s="1">
         <v>0.9</v>
       </c>
-      <c r="AH2" s="4">
+      <c r="AI2" s="4">
         <v>14</v>
       </c>
-      <c r="AI2">
+      <c r="AJ2">
         <v>4.7</v>
       </c>
-      <c r="AJ2">
+      <c r="AK2">
         <v>30</v>
       </c>
-      <c r="AK2" s="1">
+      <c r="AL2" s="1">
         <v>274</v>
       </c>
-      <c r="AL2">
+      <c r="AM2" s="3">
+        <v>16.2</v>
+      </c>
+      <c r="AN2" s="1">
+        <v>339</v>
+      </c>
+      <c r="AO2" s="4">
+        <v>70</v>
+      </c>
+      <c r="AP2" s="4">
+        <v>28</v>
+      </c>
+      <c r="AQ2" s="4">
+        <v>43</v>
+      </c>
+      <c r="AR2" s="3">
+        <v>3</v>
+      </c>
+      <c r="AS2" s="3">
+        <v>3</v>
+      </c>
+      <c r="AT2" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AU2" s="3">
+        <v>5</v>
+      </c>
+      <c r="AV2" s="4">
+        <v>30</v>
+      </c>
+      <c r="AW2" s="1">
+        <v>298</v>
+      </c>
+      <c r="AX2">
         <v>45</v>
       </c>
-      <c r="AM2">
+      <c r="AY2">
         <v>0.72</v>
       </c>
-      <c r="AN2">
+      <c r="AZ2">
+        <v>4000</v>
+      </c>
+      <c r="BA2">
+        <v>2000</v>
+      </c>
+      <c r="BB2" s="1">
+        <v>350</v>
+      </c>
+      <c r="BC2">
+        <v>0.8</v>
+      </c>
+      <c r="BD2">
+        <v>2900</v>
+      </c>
+      <c r="BE2">
         <v>1550</v>
       </c>
-      <c r="AO2" s="1">
+      <c r="BF2" s="1">
         <v>239</v>
       </c>
-      <c r="AP2">
+      <c r="BG2">
         <v>0.75</v>
       </c>
-      <c r="AQ2">
+      <c r="BH2">
         <v>21</v>
       </c>
-      <c r="AR2">
+      <c r="BI2">
         <v>30</v>
       </c>
-      <c r="AS2">
+      <c r="BJ2">
         <v>1.5</v>
       </c>
-      <c r="AT2">
+      <c r="BK2">
         <v>2.5</v>
       </c>
-      <c r="AU2">
+      <c r="BL2">
         <v>4.5</v>
       </c>
-      <c r="AV2" s="3">
+      <c r="BM2" s="3">
         <v>6</v>
       </c>
-      <c r="AW2" s="1">
+      <c r="BN2" s="1">
         <v>179</v>
       </c>
-      <c r="AX2" s="3">
+      <c r="BO2" s="3">
         <v>0.8</v>
       </c>
-      <c r="AY2">
+      <c r="BP2">
         <v>72.400000000000006</v>
       </c>
-      <c r="AZ2" s="1">
+      <c r="BQ2" s="1">
         <v>151</v>
       </c>
-      <c r="BA2">
+      <c r="BR2">
         <v>0.85</v>
       </c>
-      <c r="BB2" s="1">
+      <c r="BS2" s="1">
         <v>10.17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
econ: parameterize chainsaw productivity in long log harvests plus slope coefficients
</commit_message>
<xml_diff>
--- a/UnitTests/financial scenarios.xlsx
+++ b/UnitTests/financial scenarios.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
   <si>
     <t>name</t>
   </si>
@@ -167,18 +167,6 @@
     <t>grappleYoaderSMh</t>
   </si>
   <si>
-    <t>forwarderPMh</t>
-  </si>
-  <si>
-    <t>fellerBuncherPMh</t>
-  </si>
-  <si>
-    <t>chainsawProductivity</t>
-  </si>
-  <si>
-    <t>chainsawPMh</t>
-  </si>
-  <si>
     <t>grappleYoaderMaxPayload</t>
   </si>
   <si>
@@ -194,9 +182,6 @@
     <t>grappleSwingYarderUtilization</t>
   </si>
   <si>
-    <t>wheeledHarvesterDiameterLimit</t>
-  </si>
-  <si>
     <t>wheeledHarvesterConstant</t>
   </si>
   <si>
@@ -212,12 +197,6 @@
     <t>wheeledHarvesterSlopeThreshold</t>
   </si>
   <si>
-    <t>wheeledHarvesterPMh</t>
-  </si>
-  <si>
-    <t>trackedHarvesterDiameterLimit</t>
-  </si>
-  <si>
     <t>trackedHarvesterConstant</t>
   </si>
   <si>
@@ -227,9 +206,6 @@
     <t>trackedHarvesterSlopeThreshold</t>
   </si>
   <si>
-    <t>trackedHarvesterPMh</t>
-  </si>
-  <si>
     <t>trackedHarvesterQuadraticThreshold1</t>
   </si>
   <si>
@@ -240,15 +216,103 @@
   </si>
   <si>
     <t>trackedHarvesterQuadratic2</t>
+  </si>
+  <si>
+    <t>chainsawBuckConstant</t>
+  </si>
+  <si>
+    <t>chainsawBuckLinear</t>
+  </si>
+  <si>
+    <t>chainsawBuckQuadratic</t>
+  </si>
+  <si>
+    <t>chainsawBuckQuadraticThreshold</t>
+  </si>
+  <si>
+    <t>chainsawFellAndBuckConstant</t>
+  </si>
+  <si>
+    <t>chainsawFellAndBuckLinear</t>
+  </si>
+  <si>
+    <t>chainsawSlopeThreshold</t>
+  </si>
+  <si>
+    <t>wheeledHarvesterSMh</t>
+  </si>
+  <si>
+    <t>wheeledHarvesterUtilization</t>
+  </si>
+  <si>
+    <t>trackedHarvesterUtilization</t>
+  </si>
+  <si>
+    <t>trackedHarvesterSMh</t>
+  </si>
+  <si>
+    <t>forwarderUtilization</t>
+  </si>
+  <si>
+    <t>forwarderSMh</t>
+  </si>
+  <si>
+    <t>fellerBuncherUtilization</t>
+  </si>
+  <si>
+    <t>fellerBuncherSMh</t>
+  </si>
+  <si>
+    <t>chainsawByOperatorUtilization</t>
+  </si>
+  <si>
+    <t>chainsawByOperatorSMh</t>
+  </si>
+  <si>
+    <t>chainsawFellAndBuckUtilization</t>
+  </si>
+  <si>
+    <t>chainsawFellAndBuckSMh</t>
+  </si>
+  <si>
+    <t>chainsawBuckSMh</t>
+  </si>
+  <si>
+    <t>chainsawBuckUtilization</t>
+  </si>
+  <si>
+    <t>wheeledHarvesterSlopeLinear</t>
+  </si>
+  <si>
+    <t>chainsawSlopeLinear</t>
+  </si>
+  <si>
+    <t>fellerBuncherSlopeLinear</t>
+  </si>
+  <si>
+    <t>trackedHarvesterSlopeLinear</t>
+  </si>
+  <si>
+    <t>wheeledHarvesterFellAndBuckDiameterLimit</t>
+  </si>
+  <si>
+    <t>wheeledHarvesterFellingDiameterLimit</t>
+  </si>
+  <si>
+    <t>trackedHarvesterFellAndBuckDiameterLimit</t>
+  </si>
+  <si>
+    <t>trackedHarvesterFellingDiameterLimit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -295,13 +359,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -583,7 +648,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BS2"/>
+  <dimension ref="A1:CN2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -594,15 +659,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="14" max="14" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.33203125" customWidth="1"/>
-    <col min="17" max="17" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="18" max="31" width="11.77734375" customWidth="1"/>
-    <col min="32" max="32" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="35" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:92" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -673,151 +733,214 @@
         <v>26</v>
       </c>
       <c r="X1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG1" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AO1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AP1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AR1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AS1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AT1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AU1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AV1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AW1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="AX1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AY1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AZ1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="BA1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="BB1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="BC1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="BD1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BE1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="BF1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="BG1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="BH1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="BI1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="BJ1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BK1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="BL1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="BM1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="BN1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="BO1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="BP1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="BQ1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="BR1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="BS1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="BT1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="BU1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="BV1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="BW1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="BX1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="BY1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="Y1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC1" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="AH1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AK1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AL1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AM1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AN1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AO1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="AP1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AQ1" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="AR1" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="AS1" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AT1" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AU1" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="AV1" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AW1" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AX1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AY1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AZ1" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="BA1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="BB1" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="BC1" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="BD1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="BE1" s="2" t="s">
+      <c r="BZ1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="BF1" s="2" t="s">
+      <c r="CA1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="BG1" s="2" t="s">
+      <c r="CB1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="BH1" s="2" t="s">
+      <c r="CC1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="BI1" s="2" t="s">
+      <c r="CD1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="BJ1" s="2" t="s">
+      <c r="CE1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="BK1" s="2" t="s">
+      <c r="CF1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="BL1" s="2" t="s">
+      <c r="CG1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="BM1" s="2" t="s">
+      <c r="CH1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="BN1" s="2" t="s">
+      <c r="CI1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="BO1" s="2" t="s">
+      <c r="CJ1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="BP1" s="2" t="s">
+      <c r="CK1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="BQ1" s="2" t="s">
+      <c r="CL1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="BR1" s="2" t="s">
+      <c r="CM1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="BS1" s="2" t="s">
+      <c r="CN1" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:92" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -890,148 +1013,212 @@
         <v>66</v>
       </c>
       <c r="X2" s="1">
-        <v>258</v>
-      </c>
-      <c r="Y2" s="4">
+        <v>211.5</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>0.79</v>
+      </c>
+      <c r="Z2" s="4">
+        <v>95</v>
+      </c>
+      <c r="AA2" s="4">
         <v>70</v>
       </c>
-      <c r="Z2" s="4">
+      <c r="AB2" s="4">
         <v>28</v>
       </c>
-      <c r="AA2" s="4">
+      <c r="AC2" s="4">
         <v>43</v>
       </c>
-      <c r="AB2" s="4">
+      <c r="AD2" s="4">
         <v>6</v>
       </c>
-      <c r="AC2" s="3">
+      <c r="AE2" s="3">
         <v>1.9</v>
       </c>
-      <c r="AD2" s="4">
+      <c r="AF2" s="4">
         <v>45</v>
       </c>
-      <c r="AE2" s="1">
-        <v>308</v>
-      </c>
-      <c r="AF2" s="1">
+      <c r="AG2" s="6">
+        <v>1.15E-2</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>239.5</v>
+      </c>
+      <c r="AI2" s="1">
+        <v>0.77</v>
+      </c>
+      <c r="AJ2" s="3">
+        <v>51</v>
+      </c>
+      <c r="AK2" s="3">
+        <v>54</v>
+      </c>
+      <c r="AL2" s="4">
+        <v>30</v>
+      </c>
+      <c r="AM2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN2" s="1">
+        <v>80</v>
+      </c>
+      <c r="AO2" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="AP2" s="1">
+        <f>3.77</f>
+        <v>3.77</v>
+      </c>
+      <c r="AQ2" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="AR2" s="4">
+        <v>65</v>
+      </c>
+      <c r="AS2" s="4">
+        <v>105</v>
+      </c>
+      <c r="AT2" s="1">
+        <v>149.5</v>
+      </c>
+      <c r="AU2" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="AV2" s="4">
+        <v>50</v>
+      </c>
+      <c r="AW2" s="6">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="AX2" s="1">
         <f>65+32+3*2*(2*10+3*170)/15+25+45</f>
         <v>379</v>
       </c>
-      <c r="AG2" s="1">
+      <c r="AY2" s="1">
         <v>9.8000000000000007</v>
       </c>
-      <c r="AH2" s="1">
+      <c r="AZ2" s="1">
         <v>0.9</v>
       </c>
-      <c r="AI2" s="4">
+      <c r="BA2" s="4">
         <v>14</v>
       </c>
-      <c r="AJ2">
+      <c r="BB2">
         <v>4.7</v>
       </c>
-      <c r="AK2">
+      <c r="BC2">
         <v>30</v>
       </c>
-      <c r="AL2" s="1">
-        <v>274</v>
-      </c>
-      <c r="AM2" s="3">
-        <v>16.2</v>
-      </c>
-      <c r="AN2" s="1">
-        <v>339</v>
-      </c>
-      <c r="AO2" s="4">
-        <v>70</v>
-      </c>
-      <c r="AP2" s="4">
+      <c r="BD2" s="6">
+        <v>1.15E-2</v>
+      </c>
+      <c r="BE2" s="1">
+        <v>289.5</v>
+      </c>
+      <c r="BF2" s="1">
+        <v>0.77</v>
+      </c>
+      <c r="BG2" s="4">
+        <v>105</v>
+      </c>
+      <c r="BH2" s="4">
+        <v>80</v>
+      </c>
+      <c r="BI2" s="4">
         <v>28</v>
       </c>
-      <c r="AQ2" s="4">
+      <c r="BJ2" s="4">
         <v>43</v>
       </c>
-      <c r="AR2" s="3">
+      <c r="BK2" s="3">
         <v>3</v>
       </c>
-      <c r="AS2" s="3">
+      <c r="BL2" s="3">
         <v>3</v>
       </c>
-      <c r="AT2" s="3">
+      <c r="BM2" s="3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="AU2" s="3">
+      <c r="BN2" s="3">
         <v>5</v>
       </c>
-      <c r="AV2" s="4">
+      <c r="BO2" s="4">
         <v>30</v>
       </c>
-      <c r="AW2" s="1">
-        <v>298</v>
-      </c>
-      <c r="AX2">
+      <c r="BP2" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="BQ2" s="1">
+        <v>290.5</v>
+      </c>
+      <c r="BR2" s="1">
+        <v>0.77</v>
+      </c>
+      <c r="BS2">
         <v>45</v>
       </c>
-      <c r="AY2">
+      <c r="BT2">
         <v>0.72</v>
       </c>
-      <c r="AZ2">
+      <c r="BU2">
         <v>4000</v>
       </c>
-      <c r="BA2">
+      <c r="BV2">
         <v>2000</v>
       </c>
-      <c r="BB2" s="1">
-        <v>350</v>
-      </c>
-      <c r="BC2">
+      <c r="BW2" s="1">
+        <v>367.5</v>
+      </c>
+      <c r="BX2" s="1">
         <v>0.8</v>
       </c>
-      <c r="BD2">
+      <c r="BY2">
         <v>2900</v>
       </c>
-      <c r="BE2">
+      <c r="BZ2">
         <v>1550</v>
       </c>
-      <c r="BF2" s="1">
-        <v>239</v>
-      </c>
-      <c r="BG2">
+      <c r="CA2" s="1">
+        <v>263.5</v>
+      </c>
+      <c r="CB2">
         <v>0.75</v>
       </c>
-      <c r="BH2">
+      <c r="CC2">
         <v>21</v>
       </c>
-      <c r="BI2">
+      <c r="CD2">
         <v>30</v>
       </c>
-      <c r="BJ2">
+      <c r="CE2">
         <v>1.5</v>
       </c>
-      <c r="BK2">
+      <c r="CF2">
         <v>2.5</v>
       </c>
-      <c r="BL2">
+      <c r="CG2">
         <v>4.5</v>
       </c>
-      <c r="BM2" s="3">
+      <c r="CH2" s="3">
         <v>6</v>
       </c>
-      <c r="BN2" s="1">
-        <v>179</v>
-      </c>
-      <c r="BO2" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="BP2">
+      <c r="CI2" s="1">
+        <v>212</v>
+      </c>
+      <c r="CJ2" s="1">
+        <v>0.89</v>
+      </c>
+      <c r="CK2">
         <v>72.400000000000006</v>
       </c>
-      <c r="BQ2" s="1">
-        <v>151</v>
-      </c>
-      <c r="BR2">
-        <v>0.85</v>
-      </c>
-      <c r="BS2" s="1">
+      <c r="CL2" s="1">
+        <v>177</v>
+      </c>
+      <c r="CM2" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="CN2" s="1">
         <v>10.17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
econ: reparameterize cut to length and haul costs
</commit_message>
<xml_diff>
--- a/UnitTests/financial scenarios.xlsx
+++ b/UnitTests/financial scenarios.xlsx
@@ -12,8 +12,12 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="16188" windowHeight="7572"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="parameterization" sheetId="1" r:id="rId1"/>
+    <sheet name="tracking list" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'tracking list'!$A$1:$C$115</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="125">
   <si>
     <t>name</t>
   </si>
@@ -77,12 +81,6 @@
     <t>regenPerHa</t>
   </si>
   <si>
-    <t>regenHaulPerM3</t>
-  </si>
-  <si>
-    <t>thinHaulPerM3</t>
-  </si>
-  <si>
     <t>harvestTaxPerMbf</t>
   </si>
   <si>
@@ -303,6 +301,108 @@
   </si>
   <si>
     <t>trackedHarvesterFellingDiameterLimit</t>
+  </si>
+  <si>
+    <t>forwarderWeight</t>
+  </si>
+  <si>
+    <t>forwarderTractiveForce</t>
+  </si>
+  <si>
+    <t>ctlHaulPayload</t>
+  </si>
+  <si>
+    <t>ctlHaulHours</t>
+  </si>
+  <si>
+    <t>ctlHaulSMh</t>
+  </si>
+  <si>
+    <t>longLogHaulSMh</t>
+  </si>
+  <si>
+    <t>longLogHaulHours</t>
+  </si>
+  <si>
+    <t>longLogHaulPayload</t>
+  </si>
+  <si>
+    <t>forwarderUnloadLinearOneSort</t>
+  </si>
+  <si>
+    <t>forwarderUnloadLinearTwoSorts</t>
+  </si>
+  <si>
+    <t>forwarderUnloadLinearThreeSorts</t>
+  </si>
+  <si>
+    <t>forwarderUnloadPayload</t>
+  </si>
+  <si>
+    <t>forwarderUnloadMeanLogVolume</t>
+  </si>
+  <si>
+    <t>forwarderLoadMeanLogVolume</t>
+  </si>
+  <si>
+    <t>forwarderLoadPayload</t>
+  </si>
+  <si>
+    <t>parameter name</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>econ</t>
+  </si>
+  <si>
+    <t>wood pricing</t>
+  </si>
+  <si>
+    <t>harvest cost</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>.xlsx import</t>
+  </si>
+  <si>
+    <t>forwarderDriveWhileLoadingLinear</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>forwarderDriveWhileLoadingLogs</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>number of parameters</t>
+  </si>
+  <si>
+    <t>forwarderLoadLinear</t>
+  </si>
+  <si>
+    <t>chokerYardingLateral</t>
+  </si>
+  <si>
+    <t>chokerYardingPieces</t>
+  </si>
+  <si>
+    <t>chokerSwingYarderMaxPayload</t>
+  </si>
+  <si>
+    <t>chokerSwingYarderMeanPayload</t>
+  </si>
+  <si>
+    <t>chokerSwingYarderSMh</t>
+  </si>
+  <si>
+    <t>chokerSwingYarderUtilization</t>
   </si>
 </sst>
 </file>
@@ -359,14 +459,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -648,21 +752,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CN2"/>
+  <dimension ref="A1:DB2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AG2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="AO1" sqref="AO1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="14" max="35" width="8.88671875" customWidth="1"/>
+    <col min="14" max="45" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:92" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -694,13 +798,13 @@
         <v>6</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>16</v>
@@ -715,232 +819,274 @@
         <v>3</v>
       </c>
       <c r="R1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="T1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="V1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AO1" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ1" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="AR1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AS1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AT1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AU1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AV1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AW1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AX1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AY1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AZ1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="BA1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="BB1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="BC1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BD1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BE1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BF1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="BG1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="BH1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="BI1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="BJ1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="BK1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="BL1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="BM1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="BN1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="W1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="X1" s="2" t="s">
+      <c r="BO1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="BP1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="BQ1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="BR1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="BS1" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="BT1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="AB1" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AE1" s="5" t="s">
+      <c r="BU1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="BV1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AG1" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="AH1" s="2" t="s">
+      <c r="BW1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="BX1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="BY1" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="BZ1" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="CA1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="CB1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="CC1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="CD1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="AI1" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AK1" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="AL1" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AM1" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AN1" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AO1" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="AP1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="AQ1" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AR1" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AS1" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="AT1" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AU1" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="AV1" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="AW1" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AX1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AY1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="AZ1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="BA1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="BB1" s="2" t="s">
+      <c r="CE1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CF1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="CG1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="CH1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="CI1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="CJ1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="CK1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="CL1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="CM1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="CN1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="CO1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="BC1" s="2" t="s">
+      <c r="CP1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="BD1" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BE1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="BF1" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="BG1" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="BH1" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="BI1" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="BJ1" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="BK1" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="BL1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="BM1" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="BN1" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="BO1" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="BP1" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="BQ1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="BR1" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="BS1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="BT1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="BU1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="BV1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="BW1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="BX1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="BY1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="BZ1" s="2" t="s">
+      <c r="CQ1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="CR1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="CS1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="CT1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="CU1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="CV1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="CA1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="CB1" s="2" t="s">
+      <c r="CW1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="CX1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="CY1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="CC1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="CD1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="CE1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="CF1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="CG1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="CH1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CI1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="CJ1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="CK1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="CL1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="CM1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="CN1" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:92" x14ac:dyDescent="0.3">
+      <c r="CZ1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="DA1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="DB1" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -995,13 +1141,14 @@
         <v>728</v>
       </c>
       <c r="R2" s="4">
+        <f>23700 + 1900 + 0.5 * 2 * 2600</f>
+        <v>28200</v>
+      </c>
+      <c r="S2" s="4">
         <v>20000</v>
       </c>
-      <c r="S2" s="4">
-        <v>33</v>
-      </c>
       <c r="T2" s="4">
-        <v>45</v>
+        <v>200</v>
       </c>
       <c r="U2" s="4">
         <v>50</v>
@@ -1009,221 +1156,1592 @@
       <c r="V2" s="4">
         <v>60</v>
       </c>
-      <c r="W2" s="4">
+      <c r="W2" s="5">
+        <v>0.76980000000000004</v>
+      </c>
+      <c r="X2">
+        <v>0.97260000000000002</v>
+      </c>
+      <c r="Y2">
+        <v>0.59550000000000003</v>
+      </c>
+      <c r="Z2" s="4">
+        <v>33</v>
+      </c>
+      <c r="AA2" s="4">
+        <v>45</v>
+      </c>
+      <c r="AB2" s="4">
         <v>66</v>
       </c>
-      <c r="X2" s="1">
+      <c r="AC2" s="1">
+        <v>0.46</v>
+      </c>
+      <c r="AD2" s="1">
+        <f>1.25*0.46</f>
+        <v>0.57500000000000007</v>
+      </c>
+      <c r="AE2" s="1">
+        <f>1.75 * 0.46</f>
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="AF2" s="5">
+        <v>0.624</v>
+      </c>
+      <c r="AG2" s="5">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="AH2" s="1">
         <v>211.5</v>
       </c>
-      <c r="Y2" s="1">
+      <c r="AI2" s="1">
         <v>0.79</v>
       </c>
-      <c r="Z2" s="4">
+      <c r="AJ2" s="4">
         <v>95</v>
       </c>
-      <c r="AA2" s="4">
+      <c r="AK2" s="4">
         <v>70</v>
       </c>
-      <c r="AB2" s="4">
+      <c r="AL2" s="4">
         <v>28</v>
       </c>
-      <c r="AC2" s="4">
+      <c r="AM2" s="4">
         <v>43</v>
       </c>
-      <c r="AD2" s="4">
+      <c r="AN2" s="4">
         <v>6</v>
       </c>
-      <c r="AE2" s="3">
+      <c r="AO2" s="3">
         <v>1.9</v>
       </c>
-      <c r="AF2" s="4">
+      <c r="AP2" s="4">
         <v>45</v>
       </c>
-      <c r="AG2" s="6">
+      <c r="AQ2" s="5">
         <v>1.15E-2</v>
       </c>
-      <c r="AH2" s="1">
+      <c r="AR2" s="1">
         <v>239.5</v>
       </c>
-      <c r="AI2" s="1">
+      <c r="AS2" s="1">
         <v>0.77</v>
       </c>
-      <c r="AJ2" s="3">
+      <c r="AT2" s="3">
         <v>51</v>
       </c>
-      <c r="AK2" s="3">
+      <c r="AU2" s="3">
         <v>54</v>
       </c>
-      <c r="AL2" s="4">
+      <c r="AV2" s="4">
         <v>30</v>
       </c>
-      <c r="AM2" s="1">
+      <c r="AW2" s="1">
         <v>1</v>
       </c>
-      <c r="AN2" s="1">
+      <c r="AX2" s="1">
         <v>80</v>
       </c>
-      <c r="AO2" s="1">
+      <c r="AY2" s="1">
         <v>0.75</v>
       </c>
-      <c r="AP2" s="1">
+      <c r="AZ2" s="1">
         <f>3.77</f>
         <v>3.77</v>
       </c>
-      <c r="AQ2" s="1">
+      <c r="BA2" s="1">
         <v>0.25</v>
       </c>
-      <c r="AR2" s="4">
+      <c r="BB2" s="4">
         <v>65</v>
       </c>
-      <c r="AS2" s="4">
+      <c r="BC2" s="4">
         <v>105</v>
       </c>
-      <c r="AT2" s="1">
+      <c r="BD2" s="1">
         <v>149.5</v>
       </c>
-      <c r="AU2" s="1">
+      <c r="BE2" s="1">
         <v>0.5</v>
       </c>
-      <c r="AV2" s="4">
+      <c r="BF2" s="4">
         <v>50</v>
       </c>
-      <c r="AW2" s="6">
+      <c r="BG2" s="5">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="AX2" s="1">
+      <c r="BH2" s="1">
         <f>65+32+3*2*(2*10+3*170)/15+25+45</f>
         <v>379</v>
       </c>
-      <c r="AY2" s="1">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="AZ2" s="1">
+      <c r="BI2" s="4">
+        <f>0.99*28990</f>
+        <v>28700.1</v>
+      </c>
+      <c r="BJ2" s="1">
+        <f>(180+30+25)/60</f>
+        <v>3.9166666666666665</v>
+      </c>
+      <c r="BK2" s="1">
+        <f>3/BJ2*125</f>
+        <v>95.744680851063833</v>
+      </c>
+      <c r="BL2" s="1">
         <v>0.9</v>
       </c>
-      <c r="BA2" s="4">
+      <c r="BM2" s="4">
         <v>14</v>
       </c>
-      <c r="BB2">
+      <c r="BN2">
         <v>4.7</v>
       </c>
-      <c r="BC2">
+      <c r="BO2">
         <v>30</v>
       </c>
-      <c r="BD2" s="6">
+      <c r="BP2" s="5">
         <v>1.15E-2</v>
       </c>
-      <c r="BE2" s="1">
+      <c r="BQ2" s="1">
         <v>289.5</v>
-      </c>
-      <c r="BF2" s="1">
-        <v>0.77</v>
-      </c>
-      <c r="BG2" s="4">
-        <v>105</v>
-      </c>
-      <c r="BH2" s="4">
-        <v>80</v>
-      </c>
-      <c r="BI2" s="4">
-        <v>28</v>
-      </c>
-      <c r="BJ2" s="4">
-        <v>43</v>
-      </c>
-      <c r="BK2" s="3">
-        <v>3</v>
-      </c>
-      <c r="BL2" s="3">
-        <v>3</v>
-      </c>
-      <c r="BM2" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="BN2" s="3">
-        <v>5</v>
-      </c>
-      <c r="BO2" s="4">
-        <v>30</v>
-      </c>
-      <c r="BP2" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="BQ2" s="1">
-        <v>290.5</v>
       </c>
       <c r="BR2" s="1">
         <v>0.77</v>
       </c>
-      <c r="BS2">
+      <c r="BS2" s="4">
+        <v>105</v>
+      </c>
+      <c r="BT2" s="4">
+        <v>80</v>
+      </c>
+      <c r="BU2" s="4">
+        <v>28</v>
+      </c>
+      <c r="BV2" s="4">
+        <v>43</v>
+      </c>
+      <c r="BW2" s="3">
+        <v>3</v>
+      </c>
+      <c r="BX2" s="3">
+        <v>3</v>
+      </c>
+      <c r="BY2" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="BZ2" s="3">
+        <v>5</v>
+      </c>
+      <c r="CA2" s="4">
+        <v>30</v>
+      </c>
+      <c r="CB2" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="CC2" s="1">
+        <v>290.5</v>
+      </c>
+      <c r="CD2" s="1">
+        <v>0.77</v>
+      </c>
+      <c r="CE2">
         <v>45</v>
       </c>
-      <c r="BT2">
+      <c r="CF2">
         <v>0.72</v>
       </c>
-      <c r="BU2">
+      <c r="CG2">
         <v>4000</v>
       </c>
-      <c r="BV2">
+      <c r="CH2">
         <v>2000</v>
       </c>
-      <c r="BW2" s="1">
+      <c r="CI2" s="1">
         <v>367.5</v>
       </c>
-      <c r="BX2" s="1">
+      <c r="CJ2" s="1">
         <v>0.8</v>
       </c>
-      <c r="BY2">
+      <c r="CK2">
         <v>2900</v>
       </c>
-      <c r="BZ2">
+      <c r="CL2">
         <v>1550</v>
       </c>
-      <c r="CA2" s="1">
+      <c r="CM2" s="1">
         <v>263.5</v>
       </c>
-      <c r="CB2">
+      <c r="CN2">
         <v>0.75</v>
       </c>
-      <c r="CC2">
+      <c r="CO2">
         <v>21</v>
       </c>
-      <c r="CD2">
+      <c r="CP2">
         <v>30</v>
       </c>
-      <c r="CE2">
+      <c r="CQ2">
         <v>1.5</v>
       </c>
-      <c r="CF2">
+      <c r="CR2">
         <v>2.5</v>
       </c>
-      <c r="CG2">
+      <c r="CS2">
         <v>4.5</v>
       </c>
-      <c r="CH2" s="3">
+      <c r="CT2" s="3">
         <v>6</v>
       </c>
-      <c r="CI2" s="1">
+      <c r="CU2" s="1">
         <v>212</v>
       </c>
-      <c r="CJ2" s="1">
+      <c r="CV2" s="1">
         <v>0.89</v>
       </c>
-      <c r="CK2">
+      <c r="CW2">
         <v>72.400000000000006</v>
       </c>
-      <c r="CL2" s="1">
+      <c r="CX2" s="1">
         <v>177</v>
       </c>
-      <c r="CM2" s="1">
+      <c r="CY2" s="1">
         <v>0.9</v>
       </c>
-      <c r="CN2" s="1">
-        <v>10.17</v>
+      <c r="CZ2" s="4">
+        <f>0.99*26275</f>
+        <v>26012.25</v>
+      </c>
+      <c r="DA2" s="1">
+        <f>(180+17.5+17.5)/60</f>
+        <v>3.5833333333333335</v>
+      </c>
+      <c r="DB2" s="1">
+        <f>3/DA2*100</f>
+        <v>83.720930232558132</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F115"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A2:A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F2">
+        <f>COUNTIFS(B2:B115,E2) - 1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F3">
+        <f>COUNTIFS(B2:B115,E3)</f>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F4">
+        <f>COUNTIFS(B2:B115,E4)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E5" t="s">
+        <v>116</v>
+      </c>
+      <c r="F5">
+        <f>SUM(F2:F4)</f>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C17" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C18" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>110</v>
+      </c>
+      <c r="C20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" t="s">
+        <v>110</v>
+      </c>
+      <c r="C21" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>110</v>
+      </c>
+      <c r="C22" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" t="s">
+        <v>110</v>
+      </c>
+      <c r="C23" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B24" t="s">
+        <v>110</v>
+      </c>
+      <c r="C24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B25" t="s">
+        <v>110</v>
+      </c>
+      <c r="C25" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B26" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27" t="s">
+        <v>110</v>
+      </c>
+      <c r="C27" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B28" t="s">
+        <v>110</v>
+      </c>
+      <c r="C28" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" t="s">
+        <v>110</v>
+      </c>
+      <c r="C29" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" t="s">
+        <v>110</v>
+      </c>
+      <c r="C30" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" t="s">
+        <v>110</v>
+      </c>
+      <c r="C31" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" t="s">
+        <v>110</v>
+      </c>
+      <c r="C32" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B33" t="s">
+        <v>110</v>
+      </c>
+      <c r="C33" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B34" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B35" t="s">
+        <v>110</v>
+      </c>
+      <c r="C35" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B36" t="s">
+        <v>110</v>
+      </c>
+      <c r="C36" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" t="s">
+        <v>110</v>
+      </c>
+      <c r="C37" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" t="s">
+        <v>110</v>
+      </c>
+      <c r="C38" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B39" t="s">
+        <v>110</v>
+      </c>
+      <c r="C39" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B40" t="s">
+        <v>110</v>
+      </c>
+      <c r="C40" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41" t="s">
+        <v>110</v>
+      </c>
+      <c r="C41" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" t="s">
+        <v>110</v>
+      </c>
+      <c r="C42" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43" t="s">
+        <v>110</v>
+      </c>
+      <c r="C43" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B44" t="s">
+        <v>110</v>
+      </c>
+      <c r="C44" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B45" t="s">
+        <v>110</v>
+      </c>
+      <c r="C45" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B46" t="s">
+        <v>110</v>
+      </c>
+      <c r="C46" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B47" t="s">
+        <v>110</v>
+      </c>
+      <c r="C47" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B48" t="s">
+        <v>110</v>
+      </c>
+      <c r="C48" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B49" t="s">
+        <v>110</v>
+      </c>
+      <c r="C49" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B50" t="s">
+        <v>110</v>
+      </c>
+      <c r="C50" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B51" t="s">
+        <v>110</v>
+      </c>
+      <c r="C51" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B52" t="s">
+        <v>110</v>
+      </c>
+      <c r="C52" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B53" t="s">
+        <v>110</v>
+      </c>
+      <c r="C53" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B54" t="s">
+        <v>110</v>
+      </c>
+      <c r="C54" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B55" t="s">
+        <v>110</v>
+      </c>
+      <c r="C55" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B56" t="s">
+        <v>110</v>
+      </c>
+      <c r="C56" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B57" t="s">
+        <v>110</v>
+      </c>
+      <c r="C57" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B58" t="s">
+        <v>110</v>
+      </c>
+      <c r="C58" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B59" t="s">
+        <v>110</v>
+      </c>
+      <c r="C59" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B60" t="s">
+        <v>110</v>
+      </c>
+      <c r="C60" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B61" t="s">
+        <v>110</v>
+      </c>
+      <c r="C61" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B62" t="s">
+        <v>110</v>
+      </c>
+      <c r="C62" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B63" t="s">
+        <v>110</v>
+      </c>
+      <c r="C63" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B64" t="s">
+        <v>110</v>
+      </c>
+      <c r="C64" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B65" t="s">
+        <v>110</v>
+      </c>
+      <c r="C65" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B66" t="s">
+        <v>110</v>
+      </c>
+      <c r="C66" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B67" t="s">
+        <v>109</v>
+      </c>
+      <c r="C67" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B68" t="s">
+        <v>110</v>
+      </c>
+      <c r="C68" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B69" t="s">
+        <v>110</v>
+      </c>
+      <c r="C69" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B70" t="s">
+        <v>110</v>
+      </c>
+      <c r="C70" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B71" t="s">
+        <v>110</v>
+      </c>
+      <c r="C71" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B72" t="s">
+        <v>110</v>
+      </c>
+      <c r="C72" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B73" t="s">
+        <v>110</v>
+      </c>
+      <c r="C73" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B74" t="s">
+        <v>110</v>
+      </c>
+      <c r="C74" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B75" t="s">
+        <v>110</v>
+      </c>
+      <c r="C75" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B76" t="s">
+        <v>110</v>
+      </c>
+      <c r="C76" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B77" t="s">
+        <v>110</v>
+      </c>
+      <c r="C77" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B78" t="s">
+        <v>110</v>
+      </c>
+      <c r="C78" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B79" t="s">
+        <v>110</v>
+      </c>
+      <c r="C79" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B80" t="s">
+        <v>110</v>
+      </c>
+      <c r="C80" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B81" t="s">
+        <v>110</v>
+      </c>
+      <c r="C81" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B82" t="s">
+        <v>110</v>
+      </c>
+      <c r="C82" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B83" t="s">
+        <v>110</v>
+      </c>
+      <c r="C83" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B84" t="s">
+        <v>110</v>
+      </c>
+      <c r="C84" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B85" t="s">
+        <v>110</v>
+      </c>
+      <c r="C85" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B86" t="s">
+        <v>110</v>
+      </c>
+      <c r="C86" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B87" t="s">
+        <v>110</v>
+      </c>
+      <c r="C87" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B88" t="s">
+        <v>110</v>
+      </c>
+      <c r="C88" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B89" t="s">
+        <v>110</v>
+      </c>
+      <c r="C89" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B90" t="s">
+        <v>110</v>
+      </c>
+      <c r="C90" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B91" t="s">
+        <v>110</v>
+      </c>
+      <c r="C91" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B92" t="s">
+        <v>110</v>
+      </c>
+      <c r="C92" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B93" t="s">
+        <v>110</v>
+      </c>
+      <c r="C93" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B94" t="s">
+        <v>110</v>
+      </c>
+      <c r="C94" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B95" t="s">
+        <v>110</v>
+      </c>
+      <c r="C95" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B96" t="s">
+        <v>110</v>
+      </c>
+      <c r="C96" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B97" t="s">
+        <v>110</v>
+      </c>
+      <c r="C97" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B98" t="s">
+        <v>110</v>
+      </c>
+      <c r="C98" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B99" t="s">
+        <v>110</v>
+      </c>
+      <c r="C99" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B100" t="s">
+        <v>110</v>
+      </c>
+      <c r="C100" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B101" t="s">
+        <v>110</v>
+      </c>
+      <c r="C101" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B102" t="s">
+        <v>110</v>
+      </c>
+      <c r="C102" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B103" t="s">
+        <v>110</v>
+      </c>
+      <c r="C103" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B104" t="s">
+        <v>110</v>
+      </c>
+      <c r="C104" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A105" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B105" t="s">
+        <v>110</v>
+      </c>
+      <c r="C105" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A106" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B106" t="s">
+        <v>110</v>
+      </c>
+      <c r="C106" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B107" t="s">
+        <v>110</v>
+      </c>
+      <c r="C107" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B108" t="s">
+        <v>110</v>
+      </c>
+      <c r="C108" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B109" t="s">
+        <v>110</v>
+      </c>
+      <c r="C109" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B110" t="s">
+        <v>110</v>
+      </c>
+      <c r="C110" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B111" t="s">
+        <v>110</v>
+      </c>
+      <c r="C111" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B112" t="s">
+        <v>110</v>
+      </c>
+      <c r="C112" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B113" t="s">
+        <v>110</v>
+      </c>
+      <c r="C113" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A114" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B114" t="s">
+        <v>110</v>
+      </c>
+      <c r="C114" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A115" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B115" t="s">
+        <v>110</v>
+      </c>
+      <c r="C115" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:C115"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
econ: change loader productivity to kg/PMh₀
</commit_message>
<xml_diff>
--- a/UnitTests/financial scenarios.xlsx
+++ b/UnitTests/financial scenarios.xlsx
@@ -755,10 +755,10 @@
   <dimension ref="A1:DB2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AG2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AO1" sqref="AO1"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1397,8 +1397,9 @@
       <c r="CV2" s="1">
         <v>0.89</v>
       </c>
-      <c r="CW2">
-        <v>72.400000000000006</v>
+      <c r="CW2" s="4">
+        <f>2*CZ2</f>
+        <v>52024.5</v>
       </c>
       <c r="CX2" s="1">
         <v>177</v>

</xml_diff>

<commit_message>
logging: harvest cost and productivity
</commit_message>
<xml_diff>
--- a/UnitTests/financial scenarios.xlsx
+++ b/UnitTests/financial scenarios.xlsx
@@ -16,7 +16,7 @@
     <sheet name="tracking list" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'tracking list'!$A$1:$C$115</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'tracking list'!$A$1:$C$113</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="130">
   <si>
     <t>name</t>
   </si>
@@ -403,6 +403,21 @@
   </si>
   <si>
     <t>chokerSwingYarderUtilization</t>
+  </si>
+  <si>
+    <t>regenRoads</t>
+  </si>
+  <si>
+    <t>regenSlash</t>
+  </si>
+  <si>
+    <t>thinRoads</t>
+  </si>
+  <si>
+    <t>thinSlash</t>
+  </si>
+  <si>
+    <t>te</t>
   </si>
 </sst>
 </file>
@@ -752,7 +767,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DB2"/>
+  <dimension ref="A1:DF2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -763,10 +778,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="14" max="45" width="8.88671875" customWidth="1"/>
+    <col min="14" max="41" width="8.88671875" customWidth="1"/>
+    <col min="105" max="110" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:106" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:110" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -807,286 +823,298 @@
         <v>19</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK1" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM1" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AO1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AP1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AR1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AT1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AU1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AV1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AW1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AX1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AY1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AZ1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BA1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BB1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="BC1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="BD1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="BE1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="BF1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="BG1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="BH1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="BI1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="BJ1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BK1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="BL1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="BM1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="BN1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="BO1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="BP1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="BQ1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="BR1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="BS1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="BT1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="BU1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="BV1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="BW1" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="BX1" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="BY1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="BZ1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="CA1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="CB1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="CC1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CD1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="CE1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="CF1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="CG1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="CH1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="CI1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="CJ1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="CK1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="CL1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="CM1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="CN1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="CO1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="CP1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="CQ1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="CR1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="CS1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="CT1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="CU1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="CV1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="CW1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="CX1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="CY1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="CZ1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="DA1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="DB1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="DC1" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="DD1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="DE1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="DF1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="R1" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="AH1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="AK1" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AL1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AM1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AN1" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AO1" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="AP1" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AQ1" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="AR1" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="AS1" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="AT1" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AU1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="AV1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AW1" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="AX1" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="AY1" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AZ1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="BA1" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="BB1" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="BC1" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BD1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="BE1" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="BF1" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="BG1" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="BH1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="BI1" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="BJ1" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="BK1" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="BL1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="BM1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="BN1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="BO1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="BP1" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="BQ1" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="BR1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="BS1" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="BT1" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="BU1" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="BV1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="BW1" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="BX1" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="BY1" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="BZ1" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="CA1" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="CB1" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="CC1" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="CD1" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CE1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CF1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="CG1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="CH1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="CI1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="CJ1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="CK1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="CL1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="CM1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="CN1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="CO1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="CP1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="CQ1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="CR1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="CS1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="CT1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="CU1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="CV1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="CW1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="CX1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="CY1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="CZ1" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="DA1" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="DB1" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:106" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:110" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1126,298 +1154,311 @@
       <c r="M2">
         <v>15</v>
       </c>
-      <c r="N2" s="1">
+      <c r="N2" s="4">
+        <f>23700 + 1900 + 0.5 * 2 * 2600</f>
+        <v>28200</v>
+      </c>
+      <c r="O2" s="4">
+        <v>20000</v>
+      </c>
+      <c r="P2" s="4">
+        <v>200</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>50</v>
+      </c>
+      <c r="R2" s="4">
+        <v>60</v>
+      </c>
+      <c r="S2" s="5">
+        <v>0.76980000000000004</v>
+      </c>
+      <c r="T2">
+        <v>0.97260000000000002</v>
+      </c>
+      <c r="U2">
+        <v>0.59550000000000003</v>
+      </c>
+      <c r="V2" s="4">
+        <v>33</v>
+      </c>
+      <c r="W2" s="4">
+        <v>45</v>
+      </c>
+      <c r="X2" s="4">
+        <v>66</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>0.46</v>
+      </c>
+      <c r="Z2" s="1">
+        <f>1.25*0.46</f>
+        <v>0.57500000000000007</v>
+      </c>
+      <c r="AA2" s="1">
+        <f>1.75 * 0.46</f>
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="AB2" s="5">
+        <v>0.624</v>
+      </c>
+      <c r="AC2" s="5">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>211.5</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>0.79</v>
+      </c>
+      <c r="AF2" s="4">
+        <v>95</v>
+      </c>
+      <c r="AG2" s="4">
+        <v>70</v>
+      </c>
+      <c r="AH2" s="4">
+        <v>28</v>
+      </c>
+      <c r="AI2" s="4">
+        <v>43</v>
+      </c>
+      <c r="AJ2" s="4">
+        <v>6</v>
+      </c>
+      <c r="AK2" s="3">
+        <v>1.9</v>
+      </c>
+      <c r="AL2" s="4">
+        <v>45</v>
+      </c>
+      <c r="AM2" s="5">
+        <v>1.15E-2</v>
+      </c>
+      <c r="AN2" s="1">
+        <v>239.5</v>
+      </c>
+      <c r="AO2" s="1">
+        <v>0.77</v>
+      </c>
+      <c r="AP2" s="3">
+        <v>51</v>
+      </c>
+      <c r="AQ2" s="3">
+        <v>54</v>
+      </c>
+      <c r="AR2" s="4">
+        <v>30</v>
+      </c>
+      <c r="AS2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AT2" s="1">
+        <v>80</v>
+      </c>
+      <c r="AU2" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="AV2" s="1">
+        <f>3.77</f>
+        <v>3.77</v>
+      </c>
+      <c r="AW2" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="AX2" s="4">
+        <v>65</v>
+      </c>
+      <c r="AY2" s="4">
+        <v>105</v>
+      </c>
+      <c r="AZ2" s="1">
+        <v>149.5</v>
+      </c>
+      <c r="BA2" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="BB2" s="4">
+        <v>50</v>
+      </c>
+      <c r="BC2" s="5">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="BD2" s="4">
+        <f>0.99*28990</f>
+        <v>28700.1</v>
+      </c>
+      <c r="BE2" s="1">
+        <f>(180+30+25)/60</f>
+        <v>3.9166666666666665</v>
+      </c>
+      <c r="BF2" s="1">
+        <f>3/BE2*125</f>
+        <v>95.744680851063833</v>
+      </c>
+      <c r="BG2" s="1">
+        <f>65+32+3*2*(2*10+3*170)/15+25+45</f>
+        <v>379</v>
+      </c>
+      <c r="BH2" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="BI2" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="BJ2" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="BK2" s="4">
+        <v>14</v>
+      </c>
+      <c r="BL2">
+        <v>4.7</v>
+      </c>
+      <c r="BM2">
+        <v>30</v>
+      </c>
+      <c r="BN2" s="5">
+        <v>1.15E-2</v>
+      </c>
+      <c r="BO2" s="1">
+        <v>289.5</v>
+      </c>
+      <c r="BP2" s="1">
+        <v>0.77</v>
+      </c>
+      <c r="BQ2" s="4">
+        <v>105</v>
+      </c>
+      <c r="BR2" s="4">
+        <v>80</v>
+      </c>
+      <c r="BS2" s="4">
+        <v>28</v>
+      </c>
+      <c r="BT2" s="4">
+        <v>43</v>
+      </c>
+      <c r="BU2" s="3">
+        <v>3</v>
+      </c>
+      <c r="BV2" s="3">
+        <v>3</v>
+      </c>
+      <c r="BW2" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="BX2" s="3">
+        <v>5</v>
+      </c>
+      <c r="BY2" s="4">
+        <v>30</v>
+      </c>
+      <c r="BZ2" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="CA2" s="1">
+        <v>290.5</v>
+      </c>
+      <c r="CB2" s="1">
+        <v>0.77</v>
+      </c>
+      <c r="CC2">
+        <v>45</v>
+      </c>
+      <c r="CD2">
+        <v>0.72</v>
+      </c>
+      <c r="CE2">
+        <v>4000</v>
+      </c>
+      <c r="CF2">
+        <v>2000</v>
+      </c>
+      <c r="CG2" s="1">
+        <v>367.5</v>
+      </c>
+      <c r="CH2" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="CI2">
+        <v>2900</v>
+      </c>
+      <c r="CJ2">
+        <v>1550</v>
+      </c>
+      <c r="CK2" s="1">
+        <v>263.5</v>
+      </c>
+      <c r="CL2">
+        <v>0.75</v>
+      </c>
+      <c r="CM2">
+        <v>21</v>
+      </c>
+      <c r="CN2">
+        <v>30</v>
+      </c>
+      <c r="CO2">
+        <v>1.5</v>
+      </c>
+      <c r="CP2">
+        <v>2.5</v>
+      </c>
+      <c r="CQ2">
+        <v>4.5</v>
+      </c>
+      <c r="CR2" s="3">
+        <v>6</v>
+      </c>
+      <c r="CS2" s="1">
+        <v>212</v>
+      </c>
+      <c r="CT2" s="1">
+        <v>0.89</v>
+      </c>
+      <c r="CU2" s="4">
+        <f>2*CX2</f>
+        <v>52024.5</v>
+      </c>
+      <c r="CV2" s="1">
+        <v>177</v>
+      </c>
+      <c r="CW2" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="CX2" s="4">
+        <f>0.99*26275</f>
+        <v>26012.25</v>
+      </c>
+      <c r="CY2" s="1">
+        <f>(180+17.5+17.5)/60</f>
+        <v>3.5833333333333335</v>
+      </c>
+      <c r="CZ2" s="1">
+        <f>3/CY2*100</f>
+        <v>83.720930232558132</v>
+      </c>
+      <c r="DA2" s="1">
         <f>65+32+5*2*(2*10+3*170)/15+25+45</f>
         <v>520.33333333333326</v>
       </c>
-      <c r="O2" s="1">
+      <c r="DB2" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="DC2" s="1">
+        <f>0.35 + 0.12</f>
+        <v>0.47</v>
+      </c>
+      <c r="DD2" s="1">
         <v>275</v>
       </c>
-      <c r="P2" s="1">
+      <c r="DE2" s="1">
         <v>0.5</v>
       </c>
-      <c r="Q2" s="1">
+      <c r="DF2" s="1">
         <f>145+200+383</f>
         <v>728</v>
-      </c>
-      <c r="R2" s="4">
-        <f>23700 + 1900 + 0.5 * 2 * 2600</f>
-        <v>28200</v>
-      </c>
-      <c r="S2" s="4">
-        <v>20000</v>
-      </c>
-      <c r="T2" s="4">
-        <v>200</v>
-      </c>
-      <c r="U2" s="4">
-        <v>50</v>
-      </c>
-      <c r="V2" s="4">
-        <v>60</v>
-      </c>
-      <c r="W2" s="5">
-        <v>0.76980000000000004</v>
-      </c>
-      <c r="X2">
-        <v>0.97260000000000002</v>
-      </c>
-      <c r="Y2">
-        <v>0.59550000000000003</v>
-      </c>
-      <c r="Z2" s="4">
-        <v>33</v>
-      </c>
-      <c r="AA2" s="4">
-        <v>45</v>
-      </c>
-      <c r="AB2" s="4">
-        <v>66</v>
-      </c>
-      <c r="AC2" s="1">
-        <v>0.46</v>
-      </c>
-      <c r="AD2" s="1">
-        <f>1.25*0.46</f>
-        <v>0.57500000000000007</v>
-      </c>
-      <c r="AE2" s="1">
-        <f>1.75 * 0.46</f>
-        <v>0.80500000000000005</v>
-      </c>
-      <c r="AF2" s="5">
-        <v>0.624</v>
-      </c>
-      <c r="AG2" s="5">
-        <v>0.48599999999999999</v>
-      </c>
-      <c r="AH2" s="1">
-        <v>211.5</v>
-      </c>
-      <c r="AI2" s="1">
-        <v>0.79</v>
-      </c>
-      <c r="AJ2" s="4">
-        <v>95</v>
-      </c>
-      <c r="AK2" s="4">
-        <v>70</v>
-      </c>
-      <c r="AL2" s="4">
-        <v>28</v>
-      </c>
-      <c r="AM2" s="4">
-        <v>43</v>
-      </c>
-      <c r="AN2" s="4">
-        <v>6</v>
-      </c>
-      <c r="AO2" s="3">
-        <v>1.9</v>
-      </c>
-      <c r="AP2" s="4">
-        <v>45</v>
-      </c>
-      <c r="AQ2" s="5">
-        <v>1.15E-2</v>
-      </c>
-      <c r="AR2" s="1">
-        <v>239.5</v>
-      </c>
-      <c r="AS2" s="1">
-        <v>0.77</v>
-      </c>
-      <c r="AT2" s="3">
-        <v>51</v>
-      </c>
-      <c r="AU2" s="3">
-        <v>54</v>
-      </c>
-      <c r="AV2" s="4">
-        <v>30</v>
-      </c>
-      <c r="AW2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AX2" s="1">
-        <v>80</v>
-      </c>
-      <c r="AY2" s="1">
-        <v>0.75</v>
-      </c>
-      <c r="AZ2" s="1">
-        <f>3.77</f>
-        <v>3.77</v>
-      </c>
-      <c r="BA2" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="BB2" s="4">
-        <v>65</v>
-      </c>
-      <c r="BC2" s="4">
-        <v>105</v>
-      </c>
-      <c r="BD2" s="1">
-        <v>149.5</v>
-      </c>
-      <c r="BE2" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="BF2" s="4">
-        <v>50</v>
-      </c>
-      <c r="BG2" s="5">
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="BH2" s="1">
-        <f>65+32+3*2*(2*10+3*170)/15+25+45</f>
-        <v>379</v>
-      </c>
-      <c r="BI2" s="4">
-        <f>0.99*28990</f>
-        <v>28700.1</v>
-      </c>
-      <c r="BJ2" s="1">
-        <f>(180+30+25)/60</f>
-        <v>3.9166666666666665</v>
-      </c>
-      <c r="BK2" s="1">
-        <f>3/BJ2*125</f>
-        <v>95.744680851063833</v>
-      </c>
-      <c r="BL2" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="BM2" s="4">
-        <v>14</v>
-      </c>
-      <c r="BN2">
-        <v>4.7</v>
-      </c>
-      <c r="BO2">
-        <v>30</v>
-      </c>
-      <c r="BP2" s="5">
-        <v>1.15E-2</v>
-      </c>
-      <c r="BQ2" s="1">
-        <v>289.5</v>
-      </c>
-      <c r="BR2" s="1">
-        <v>0.77</v>
-      </c>
-      <c r="BS2" s="4">
-        <v>105</v>
-      </c>
-      <c r="BT2" s="4">
-        <v>80</v>
-      </c>
-      <c r="BU2" s="4">
-        <v>28</v>
-      </c>
-      <c r="BV2" s="4">
-        <v>43</v>
-      </c>
-      <c r="BW2" s="3">
-        <v>3</v>
-      </c>
-      <c r="BX2" s="3">
-        <v>3</v>
-      </c>
-      <c r="BY2" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="BZ2" s="3">
-        <v>5</v>
-      </c>
-      <c r="CA2" s="4">
-        <v>30</v>
-      </c>
-      <c r="CB2" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="CC2" s="1">
-        <v>290.5</v>
-      </c>
-      <c r="CD2" s="1">
-        <v>0.77</v>
-      </c>
-      <c r="CE2">
-        <v>45</v>
-      </c>
-      <c r="CF2">
-        <v>0.72</v>
-      </c>
-      <c r="CG2">
-        <v>4000</v>
-      </c>
-      <c r="CH2">
-        <v>2000</v>
-      </c>
-      <c r="CI2" s="1">
-        <v>367.5</v>
-      </c>
-      <c r="CJ2" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="CK2">
-        <v>2900</v>
-      </c>
-      <c r="CL2">
-        <v>1550</v>
-      </c>
-      <c r="CM2" s="1">
-        <v>263.5</v>
-      </c>
-      <c r="CN2">
-        <v>0.75</v>
-      </c>
-      <c r="CO2">
-        <v>21</v>
-      </c>
-      <c r="CP2">
-        <v>30</v>
-      </c>
-      <c r="CQ2">
-        <v>1.5</v>
-      </c>
-      <c r="CR2">
-        <v>2.5</v>
-      </c>
-      <c r="CS2">
-        <v>4.5</v>
-      </c>
-      <c r="CT2" s="3">
-        <v>6</v>
-      </c>
-      <c r="CU2" s="1">
-        <v>212</v>
-      </c>
-      <c r="CV2" s="1">
-        <v>0.89</v>
-      </c>
-      <c r="CW2" s="4">
-        <f>2*CZ2</f>
-        <v>52024.5</v>
-      </c>
-      <c r="CX2" s="1">
-        <v>177</v>
-      </c>
-      <c r="CY2" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="CZ2" s="4">
-        <f>0.99*26275</f>
-        <v>26012.25</v>
-      </c>
-      <c r="DA2" s="1">
-        <f>(180+17.5+17.5)/60</f>
-        <v>3.5833333333333335</v>
-      </c>
-      <c r="DB2" s="1">
-        <f>3/DA2*100</f>
-        <v>83.720930232558132</v>
       </c>
     </row>
   </sheetData>
@@ -1428,11 +1469,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F115"/>
+  <dimension ref="A1:F119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A2:A13"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1472,7 +1513,7 @@
         <v>108</v>
       </c>
       <c r="F2">
-        <f>COUNTIFS(B2:B115,E2) - 1</f>
+        <f>COUNTIFS(B2:B119,E2) - 1</f>
         <v>3</v>
       </c>
     </row>
@@ -1490,8 +1531,8 @@
         <v>110</v>
       </c>
       <c r="F3">
-        <f>COUNTIFS(B2:B115,E3)</f>
-        <v>101</v>
+        <f>COUNTIFS(B2:B119,E3)</f>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1508,7 +1549,7 @@
         <v>109</v>
       </c>
       <c r="F4">
-        <f>COUNTIFS(B2:B115,E4)</f>
+        <f>COUNTIFS(B2:B119,E4)</f>
         <v>9</v>
       </c>
     </row>
@@ -1527,7 +1568,7 @@
       </c>
       <c r="F5">
         <f>SUM(F2:F4)</f>
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1631,7 +1672,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="B15" t="s">
         <v>110</v>
@@ -1642,7 +1683,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
         <v>110</v>
@@ -1653,7 +1694,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>5</v>
+        <v>92</v>
       </c>
       <c r="B17" t="s">
         <v>110</v>
@@ -1664,7 +1705,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
         <v>110</v>
@@ -1675,7 +1716,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>91</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
         <v>110</v>
@@ -1686,18 +1727,18 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>20</v>
+        <v>113</v>
       </c>
       <c r="B20" t="s">
         <v>110</v>
       </c>
       <c r="C20" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>92</v>
+        <v>115</v>
       </c>
       <c r="B21" t="s">
         <v>110</v>
@@ -1708,18 +1749,18 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>23</v>
+        <v>118</v>
       </c>
       <c r="B22" t="s">
         <v>110</v>
       </c>
       <c r="C22" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>25</v>
+        <v>105</v>
       </c>
       <c r="B23" t="s">
         <v>110</v>
@@ -1730,18 +1771,18 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="B24" t="s">
         <v>110</v>
       </c>
       <c r="C24" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>115</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
         <v>110</v>
@@ -1752,18 +1793,18 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
-        <v>118</v>
+        <v>22</v>
       </c>
       <c r="B26" t="s">
         <v>110</v>
       </c>
       <c r="C26" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
-        <v>105</v>
+        <v>24</v>
       </c>
       <c r="B27" t="s">
         <v>110</v>
@@ -1774,7 +1815,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B28" t="s">
         <v>110</v>
@@ -1785,7 +1826,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
-        <v>21</v>
+        <v>100</v>
       </c>
       <c r="B29" t="s">
         <v>110</v>
@@ -1796,7 +1837,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
-        <v>22</v>
+        <v>101</v>
       </c>
       <c r="B30" t="s">
         <v>110</v>
@@ -1807,7 +1848,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
-        <v>24</v>
+        <v>102</v>
       </c>
       <c r="B31" t="s">
         <v>110</v>
@@ -1818,7 +1859,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B32" t="s">
         <v>110</v>
@@ -1829,7 +1870,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="B33" t="s">
         <v>110</v>
@@ -1840,7 +1881,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="B34" t="s">
         <v>110</v>
@@ -1851,7 +1892,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="B35" t="s">
         <v>110</v>
@@ -1862,7 +1903,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="B36" t="s">
         <v>110</v>
@@ -1873,7 +1914,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="B37" t="s">
         <v>110</v>
@@ -1884,7 +1925,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="B38" t="s">
         <v>110</v>
@@ -1895,7 +1936,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
-        <v>88</v>
+        <v>52</v>
       </c>
       <c r="B39" t="s">
         <v>110</v>
@@ -1905,8 +1946,8 @@
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="6" t="s">
-        <v>87</v>
+      <c r="A40" s="7" t="s">
+        <v>53</v>
       </c>
       <c r="B40" t="s">
         <v>110</v>
@@ -1917,7 +1958,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B41" t="s">
         <v>110</v>
@@ -1927,8 +1968,8 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="6" t="s">
-        <v>51</v>
+      <c r="A42" s="7" t="s">
+        <v>83</v>
       </c>
       <c r="B42" t="s">
         <v>110</v>
@@ -1939,7 +1980,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="B43" t="s">
         <v>110</v>
@@ -1949,8 +1990,8 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="7" t="s">
-        <v>53</v>
+      <c r="A44" s="6" t="s">
+        <v>70</v>
       </c>
       <c r="B44" t="s">
         <v>110</v>
@@ -1961,7 +2002,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B45" t="s">
         <v>110</v>
@@ -1971,8 +2012,8 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="7" t="s">
-        <v>83</v>
+      <c r="A46" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="B46" t="s">
         <v>110</v>
@@ -1983,7 +2024,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B47" t="s">
         <v>110</v>
@@ -1994,7 +2035,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B48" t="s">
         <v>110</v>
@@ -2005,7 +2046,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="B49" t="s">
         <v>110</v>
@@ -2016,7 +2057,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="B50" t="s">
         <v>110</v>
@@ -2027,7 +2068,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="B51" t="s">
         <v>110</v>
@@ -2038,7 +2079,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="B52" t="s">
         <v>110</v>
@@ -2049,7 +2090,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="B53" t="s">
         <v>110</v>
@@ -2060,7 +2101,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="B54" t="s">
         <v>110</v>
@@ -2071,7 +2112,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B55" t="s">
         <v>110</v>
@@ -2082,7 +2123,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B56" t="s">
         <v>110</v>
@@ -2093,7 +2134,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B57" t="s">
         <v>110</v>
@@ -2104,7 +2145,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="B58" t="s">
         <v>110</v>
@@ -2115,7 +2156,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="B59" t="s">
         <v>110</v>
@@ -2126,7 +2167,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="B60" t="s">
         <v>110</v>
@@ -2137,7 +2178,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
       <c r="B61" t="s">
         <v>110</v>
@@ -2148,7 +2189,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="6" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="B62" t="s">
         <v>110</v>
@@ -2159,10 +2200,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B63" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C63" t="s">
         <v>111</v>
@@ -2170,7 +2211,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="6" t="s">
-        <v>93</v>
+        <v>127</v>
       </c>
       <c r="B64" t="s">
         <v>110</v>
@@ -2181,7 +2222,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="6" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="B65" t="s">
         <v>110</v>
@@ -2192,7 +2233,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="6" t="s">
-        <v>95</v>
+        <v>26</v>
       </c>
       <c r="B66" t="s">
         <v>110</v>
@@ -2203,10 +2244,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="6" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="B67" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C67" t="s">
         <v>111</v>
@@ -2214,7 +2255,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B68" t="s">
         <v>110</v>
@@ -2225,7 +2266,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="6" t="s">
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="B69" t="s">
         <v>110</v>
@@ -2236,7 +2277,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="6" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="B70" t="s">
         <v>110</v>
@@ -2247,7 +2288,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B71" t="s">
         <v>110</v>
@@ -2258,7 +2299,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="6" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="B72" t="s">
         <v>110</v>
@@ -2269,7 +2310,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="6" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="B73" t="s">
         <v>110</v>
@@ -2280,7 +2321,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="6" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="B74" t="s">
         <v>110</v>
@@ -2291,7 +2332,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="6" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="B75" t="s">
         <v>110</v>
@@ -2302,7 +2343,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="6" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B76" t="s">
         <v>110</v>
@@ -2313,7 +2354,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="6" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B77" t="s">
         <v>110</v>
@@ -2323,8 +2364,8 @@
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" s="6" t="s">
-        <v>60</v>
+      <c r="A78" s="8" t="s">
+        <v>58</v>
       </c>
       <c r="B78" t="s">
         <v>110</v>
@@ -2334,8 +2375,8 @@
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A79" s="6" t="s">
-        <v>61</v>
+      <c r="A79" s="9" t="s">
+        <v>59</v>
       </c>
       <c r="B79" t="s">
         <v>110</v>
@@ -2345,8 +2386,8 @@
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A80" s="8" t="s">
-        <v>58</v>
+      <c r="A80" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="B80" t="s">
         <v>110</v>
@@ -2356,8 +2397,8 @@
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A81" s="9" t="s">
-        <v>59</v>
+      <c r="A81" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="B81" t="s">
         <v>110</v>
@@ -2368,7 +2409,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="6" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="B82" t="s">
         <v>110</v>
@@ -2379,7 +2420,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="6" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="B83" t="s">
         <v>110</v>
@@ -2390,29 +2431,29 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="6" t="s">
-        <v>72</v>
+        <v>119</v>
       </c>
       <c r="B84" t="s">
         <v>110</v>
       </c>
       <c r="C84" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="6" t="s">
-        <v>71</v>
+        <v>120</v>
       </c>
       <c r="B85" t="s">
         <v>110</v>
       </c>
       <c r="C85" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="6" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B86" t="s">
         <v>110</v>
@@ -2423,7 +2464,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="6" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B87" t="s">
         <v>110</v>
@@ -2434,7 +2475,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="6" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B88" t="s">
         <v>110</v>
@@ -2445,7 +2486,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="6" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B89" t="s">
         <v>110</v>
@@ -2456,29 +2497,29 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="6" t="s">
-        <v>123</v>
+        <v>36</v>
       </c>
       <c r="B90" t="s">
         <v>110</v>
       </c>
       <c r="C90" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="6" t="s">
-        <v>124</v>
+        <v>37</v>
       </c>
       <c r="B91" t="s">
         <v>110</v>
       </c>
       <c r="C91" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="6" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="B92" t="s">
         <v>110</v>
@@ -2489,7 +2530,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="6" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B93" t="s">
         <v>110</v>
@@ -2500,7 +2541,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B94" t="s">
         <v>110</v>
@@ -2511,7 +2552,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B95" t="s">
         <v>110</v>
@@ -2522,7 +2563,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B96" t="s">
         <v>110</v>
@@ -2533,7 +2574,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="6" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B97" t="s">
         <v>110</v>
@@ -2544,7 +2585,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B98" t="s">
         <v>110</v>
@@ -2555,7 +2596,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B99" t="s">
         <v>110</v>
@@ -2566,7 +2607,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="6" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="B100" t="s">
         <v>110</v>
@@ -2577,7 +2618,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="6" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B101" t="s">
         <v>110</v>
@@ -2588,7 +2629,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B102" t="s">
         <v>110</v>
@@ -2599,7 +2640,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B103" t="s">
         <v>110</v>
@@ -2610,7 +2651,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B104" t="s">
         <v>110</v>
@@ -2621,7 +2662,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B105" t="s">
         <v>110</v>
@@ -2632,7 +2673,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="6" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B106" t="s">
         <v>110</v>
@@ -2643,7 +2684,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="6" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B107" t="s">
         <v>110</v>
@@ -2654,7 +2695,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="6" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B108" t="s">
         <v>110</v>
@@ -2665,7 +2706,7 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B109" t="s">
         <v>110</v>
@@ -2676,7 +2717,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B110" t="s">
         <v>110</v>
@@ -2687,7 +2728,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="6" t="s">
-        <v>42</v>
+        <v>98</v>
       </c>
       <c r="B111" t="s">
         <v>110</v>
@@ -2698,7 +2739,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="6" t="s">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="B112" t="s">
         <v>110</v>
@@ -2709,7 +2750,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B113" t="s">
         <v>110</v>
@@ -2720,7 +2761,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="6" t="s">
-        <v>97</v>
+        <v>16</v>
       </c>
       <c r="B114" t="s">
         <v>110</v>
@@ -2731,7 +2772,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="6" t="s">
-        <v>96</v>
+        <v>125</v>
       </c>
       <c r="B115" t="s">
         <v>110</v>
@@ -2740,8 +2781,52 @@
         <v>111</v>
       </c>
     </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A116" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B116" t="s">
+        <v>110</v>
+      </c>
+      <c r="C116" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A117" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B117" t="s">
+        <v>110</v>
+      </c>
+      <c r="C117" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A118" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B118" t="s">
+        <v>110</v>
+      </c>
+      <c r="C118" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A119" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B119" t="s">
+        <v>110</v>
+      </c>
+      <c r="C119" t="s">
+        <v>111</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C115"/>
+  <autoFilter ref="A1:C119"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
econ: adjust machine costs for cardlock off road diesel
</commit_message>
<xml_diff>
--- a/UnitTests/financial scenarios.xlsx
+++ b/UnitTests/financial scenarios.xlsx
@@ -770,15 +770,15 @@
   <dimension ref="A1:DF2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AZ2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="BG2" sqref="BG2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="14" max="41" width="8.88671875" customWidth="1"/>
+    <col min="14" max="23" width="8.88671875" customWidth="1"/>
     <col min="105" max="110" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -823,133 +823,133 @@
         <v>19</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AM1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="AU1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="AV1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="BA1" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="BB1" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="BC1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="BD1" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AH1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AK1" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="AL1" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AM1" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="AN1" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="AO1" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="AP1" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AQ1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="AR1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AS1" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="AT1" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="AU1" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AV1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AW1" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AX1" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AY1" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AZ1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="BA1" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="BB1" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="BC1" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="BD1" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="BE1" s="2" t="s">
         <v>94</v>
@@ -1155,138 +1155,137 @@
         <v>15</v>
       </c>
       <c r="N2" s="4">
+        <v>95</v>
+      </c>
+      <c r="O2" s="4">
+        <v>70</v>
+      </c>
+      <c r="P2" s="4">
+        <v>28</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>43</v>
+      </c>
+      <c r="R2" s="4">
+        <v>6</v>
+      </c>
+      <c r="S2" s="3">
+        <v>1.9</v>
+      </c>
+      <c r="T2" s="4">
+        <v>45</v>
+      </c>
+      <c r="U2" s="5">
+        <v>1.15E-2</v>
+      </c>
+      <c r="V2" s="1">
+        <v>225</v>
+      </c>
+      <c r="W2" s="1">
+        <v>0.77</v>
+      </c>
+      <c r="X2" s="3">
+        <v>51</v>
+      </c>
+      <c r="Y2" s="3">
+        <v>54</v>
+      </c>
+      <c r="Z2" s="4">
+        <v>30</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>80</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>2.17</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="AF2" s="4">
+        <v>65</v>
+      </c>
+      <c r="AG2" s="4">
+        <v>105</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>149.5</v>
+      </c>
+      <c r="AI2" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="AJ2" s="4">
+        <v>50</v>
+      </c>
+      <c r="AK2" s="5">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="AL2" s="4">
+        <f>0.99*28990</f>
+        <v>28700.1</v>
+      </c>
+      <c r="AM2" s="4">
         <f>23700 + 1900 + 0.5 * 2 * 2600</f>
         <v>28200</v>
       </c>
-      <c r="O2" s="4">
+      <c r="AN2" s="4">
         <v>20000</v>
       </c>
-      <c r="P2" s="4">
+      <c r="AO2" s="4">
         <v>200</v>
       </c>
-      <c r="Q2" s="4">
+      <c r="AP2" s="4">
         <v>50</v>
       </c>
-      <c r="R2" s="4">
+      <c r="AQ2" s="4">
         <v>60</v>
       </c>
-      <c r="S2" s="5">
+      <c r="AR2" s="5">
         <v>0.76980000000000004</v>
       </c>
-      <c r="T2">
+      <c r="AS2">
         <v>0.97260000000000002</v>
       </c>
-      <c r="U2">
+      <c r="AT2">
         <v>0.59550000000000003</v>
       </c>
-      <c r="V2" s="4">
+      <c r="AU2" s="4">
         <v>33</v>
       </c>
-      <c r="W2" s="4">
+      <c r="AV2" s="4">
         <v>45</v>
       </c>
-      <c r="X2" s="4">
+      <c r="AW2" s="4">
         <v>66</v>
       </c>
-      <c r="Y2" s="1">
+      <c r="AX2" s="1">
         <v>0.46</v>
       </c>
-      <c r="Z2" s="1">
+      <c r="AY2" s="1">
         <f>1.25*0.46</f>
         <v>0.57500000000000007</v>
       </c>
-      <c r="AA2" s="1">
+      <c r="AZ2" s="1">
         <f>1.75 * 0.46</f>
         <v>0.80500000000000005</v>
       </c>
-      <c r="AB2" s="5">
+      <c r="BA2" s="5">
         <v>0.624</v>
       </c>
-      <c r="AC2" s="5">
+      <c r="BB2" s="5">
         <v>0.48599999999999999</v>
       </c>
-      <c r="AD2" s="1">
-        <v>211.5</v>
-      </c>
-      <c r="AE2" s="1">
+      <c r="BC2" s="1">
+        <v>200</v>
+      </c>
+      <c r="BD2" s="1">
         <v>0.79</v>
-      </c>
-      <c r="AF2" s="4">
-        <v>95</v>
-      </c>
-      <c r="AG2" s="4">
-        <v>70</v>
-      </c>
-      <c r="AH2" s="4">
-        <v>28</v>
-      </c>
-      <c r="AI2" s="4">
-        <v>43</v>
-      </c>
-      <c r="AJ2" s="4">
-        <v>6</v>
-      </c>
-      <c r="AK2" s="3">
-        <v>1.9</v>
-      </c>
-      <c r="AL2" s="4">
-        <v>45</v>
-      </c>
-      <c r="AM2" s="5">
-        <v>1.15E-2</v>
-      </c>
-      <c r="AN2" s="1">
-        <v>239.5</v>
-      </c>
-      <c r="AO2" s="1">
-        <v>0.77</v>
-      </c>
-      <c r="AP2" s="3">
-        <v>51</v>
-      </c>
-      <c r="AQ2" s="3">
-        <v>54</v>
-      </c>
-      <c r="AR2" s="4">
-        <v>30</v>
-      </c>
-      <c r="AS2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AT2" s="1">
-        <v>80</v>
-      </c>
-      <c r="AU2" s="1">
-        <v>0.75</v>
-      </c>
-      <c r="AV2" s="1">
-        <f>3.77</f>
-        <v>3.77</v>
-      </c>
-      <c r="AW2" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="AX2" s="4">
-        <v>65</v>
-      </c>
-      <c r="AY2" s="4">
-        <v>105</v>
-      </c>
-      <c r="AZ2" s="1">
-        <v>149.5</v>
-      </c>
-      <c r="BA2" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="BB2" s="4">
-        <v>50</v>
-      </c>
-      <c r="BC2" s="5">
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="BD2" s="4">
-        <f>0.99*28990</f>
-        <v>28700.1</v>
       </c>
       <c r="BE2" s="1">
         <f>(180+30+25)/60</f>
@@ -1322,7 +1321,7 @@
         <v>1.15E-2</v>
       </c>
       <c r="BO2" s="1">
-        <v>289.5</v>
+        <v>263</v>
       </c>
       <c r="BP2" s="1">
         <v>0.77</v>
@@ -1358,7 +1357,7 @@
         <v>0.01</v>
       </c>
       <c r="CA2" s="1">
-        <v>290.5</v>
+        <v>264</v>
       </c>
       <c r="CB2" s="1">
         <v>0.77</v>
@@ -1376,7 +1375,7 @@
         <v>2000</v>
       </c>
       <c r="CG2" s="1">
-        <v>367.5</v>
+        <v>360</v>
       </c>
       <c r="CH2" s="1">
         <v>0.8</v>
@@ -1388,7 +1387,7 @@
         <v>1550</v>
       </c>
       <c r="CK2" s="1">
-        <v>263.5</v>
+        <v>248</v>
       </c>
       <c r="CL2">
         <v>0.75</v>
@@ -1412,7 +1411,7 @@
         <v>6</v>
       </c>
       <c r="CS2" s="1">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="CT2" s="1">
         <v>0.89</v>
@@ -1422,7 +1421,7 @@
         <v>52024.5</v>
       </c>
       <c r="CV2" s="1">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="CW2" s="1">
         <v>0.9</v>

</xml_diff>

<commit_message>
econ: parameterize machine move in and out cost
</commit_message>
<xml_diff>
--- a/UnitTests/financial scenarios.xlsx
+++ b/UnitTests/financial scenarios.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="132">
   <si>
     <t>name</t>
   </si>
@@ -418,6 +418,12 @@
   </si>
   <si>
     <t>te</t>
+  </si>
+  <si>
+    <t>machineInOut</t>
+  </si>
+  <si>
+    <t>sitePrepPlant</t>
   </si>
 </sst>
 </file>
@@ -767,22 +773,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DF2"/>
+  <dimension ref="A1:DG2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AZ2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="CZ2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BG2" sqref="BG2"/>
+      <selection pane="bottomRight" activeCell="DE1" sqref="DE1:DG2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="14" max="23" width="8.88671875" customWidth="1"/>
-    <col min="105" max="110" width="8.88671875" customWidth="1"/>
+    <col min="15" max="24" width="8.88671875" customWidth="1"/>
+    <col min="106" max="111" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:110" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:111" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -820,301 +826,304 @@
         <v>17</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="T1" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="V1" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AU1" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AV1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="AY1" s="2" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="BA1" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="BA1" s="2" t="s">
+      <c r="BB1" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="BB1" s="2" t="s">
+      <c r="BC1" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="BC1" s="2" t="s">
+      <c r="BD1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="BD1" s="2" t="s">
+      <c r="BE1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="BE1" s="2" t="s">
+      <c r="BF1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="BF1" s="2" t="s">
+      <c r="BG1" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="BG1" s="2" t="s">
+      <c r="BH1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="BH1" s="2" t="s">
+      <c r="BI1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="BI1" s="2" t="s">
+      <c r="BJ1" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="BJ1" s="2" t="s">
+      <c r="BK1" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="BK1" s="2" t="s">
+      <c r="BL1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="BL1" s="2" t="s">
+      <c r="BM1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="BM1" s="2" t="s">
+      <c r="BN1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="BN1" s="2" t="s">
+      <c r="BO1" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="BO1" s="2" t="s">
+      <c r="BP1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="BP1" s="2" t="s">
+      <c r="BQ1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="BQ1" s="2" t="s">
+      <c r="BR1" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="BR1" s="2" t="s">
+      <c r="BS1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="BS1" s="2" t="s">
+      <c r="BT1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="BT1" s="2" t="s">
+      <c r="BU1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="BU1" s="2" t="s">
+      <c r="BV1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="BV1" s="2" t="s">
+      <c r="BW1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="BW1" s="10" t="s">
+      <c r="BX1" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="BX1" s="10" t="s">
+      <c r="BY1" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="BY1" s="2" t="s">
+      <c r="BZ1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="BZ1" s="2" t="s">
+      <c r="CA1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="CA1" s="2" t="s">
+      <c r="CB1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="CB1" s="2" t="s">
+      <c r="CC1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="CC1" s="2" t="s">
+      <c r="CD1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="CD1" s="2" t="s">
+      <c r="CE1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="CE1" s="2" t="s">
+      <c r="CF1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="CF1" s="2" t="s">
+      <c r="CG1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="CG1" s="2" t="s">
+      <c r="CH1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="CH1" s="2" t="s">
+      <c r="CI1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="CI1" s="2" t="s">
+      <c r="CJ1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="CJ1" s="2" t="s">
+      <c r="CK1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="CK1" s="2" t="s">
+      <c r="CL1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="CL1" s="2" t="s">
+      <c r="CM1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="CM1" s="2" t="s">
+      <c r="CN1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="CN1" s="2" t="s">
+      <c r="CO1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="CO1" s="2" t="s">
+      <c r="CP1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="CP1" s="2" t="s">
+      <c r="CQ1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="CQ1" s="2" t="s">
+      <c r="CR1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="CR1" s="2" t="s">
+      <c r="CS1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="CS1" s="2" t="s">
+      <c r="CT1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="CT1" s="2" t="s">
+      <c r="CU1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="CU1" s="2" t="s">
+      <c r="CV1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="CV1" s="2" t="s">
+      <c r="CW1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="CW1" s="2" t="s">
+      <c r="CX1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="CX1" s="2" t="s">
+      <c r="CY1" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="CY1" s="2" t="s">
+      <c r="CZ1" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="CZ1" s="2" t="s">
+      <c r="DA1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="DA1" s="2" t="s">
+      <c r="DB1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="DB1" s="2" t="s">
+      <c r="DC1" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="DC1" s="2" t="s">
+      <c r="DD1" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="DD1" s="2" t="s">
+      <c r="DE1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="DF1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="DG1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="DE1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="DF1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:110" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:111" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1152,312 +1161,316 @@
         <v>4.1322000000000001</v>
       </c>
       <c r="M2">
+        <f>2*10+3*170</f>
+        <v>530</v>
+      </c>
+      <c r="N2">
         <v>15</v>
       </c>
-      <c r="N2" s="4">
+      <c r="O2" s="4">
         <v>95</v>
       </c>
-      <c r="O2" s="4">
+      <c r="P2" s="4">
         <v>70</v>
       </c>
-      <c r="P2" s="4">
+      <c r="Q2" s="4">
         <v>28</v>
       </c>
-      <c r="Q2" s="4">
+      <c r="R2" s="4">
         <v>43</v>
       </c>
-      <c r="R2" s="4">
+      <c r="S2" s="4">
         <v>6</v>
       </c>
-      <c r="S2" s="3">
+      <c r="T2" s="3">
         <v>1.9</v>
       </c>
-      <c r="T2" s="4">
+      <c r="U2" s="4">
         <v>45</v>
       </c>
-      <c r="U2" s="5">
+      <c r="V2" s="5">
         <v>1.15E-2</v>
       </c>
-      <c r="V2" s="1">
+      <c r="W2" s="1">
         <v>225</v>
       </c>
-      <c r="W2" s="1">
+      <c r="X2" s="1">
         <v>0.77</v>
       </c>
-      <c r="X2" s="3">
+      <c r="Y2" s="3">
         <v>51</v>
       </c>
-      <c r="Y2" s="3">
+      <c r="Z2" s="3">
         <v>54</v>
       </c>
-      <c r="Z2" s="4">
+      <c r="AA2" s="4">
         <v>30</v>
       </c>
-      <c r="AA2" s="1">
+      <c r="AB2" s="1">
         <v>1</v>
       </c>
-      <c r="AB2" s="1">
+      <c r="AC2" s="1">
         <v>80</v>
       </c>
-      <c r="AC2" s="1">
+      <c r="AD2" s="1">
         <v>0.75</v>
       </c>
-      <c r="AD2" s="1">
+      <c r="AE2" s="1">
         <v>2.17</v>
       </c>
-      <c r="AE2" s="1">
+      <c r="AF2" s="1">
         <v>0.25</v>
       </c>
-      <c r="AF2" s="4">
+      <c r="AG2" s="4">
         <v>65</v>
       </c>
-      <c r="AG2" s="4">
+      <c r="AH2" s="4">
         <v>105</v>
       </c>
-      <c r="AH2" s="1">
+      <c r="AI2" s="1">
         <v>149.5</v>
       </c>
-      <c r="AI2" s="1">
+      <c r="AJ2" s="1">
         <v>0.5</v>
       </c>
-      <c r="AJ2" s="4">
+      <c r="AK2" s="4">
         <v>50</v>
       </c>
-      <c r="AK2" s="5">
+      <c r="AL2" s="5">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="AL2" s="4">
+      <c r="AM2" s="4">
         <f>0.99*28990</f>
         <v>28700.1</v>
       </c>
-      <c r="AM2" s="4">
+      <c r="AN2" s="4">
         <f>23700 + 1900 + 0.5 * 2 * 2600</f>
         <v>28200</v>
       </c>
-      <c r="AN2" s="4">
+      <c r="AO2" s="4">
         <v>20000</v>
       </c>
-      <c r="AO2" s="4">
+      <c r="AP2" s="4">
         <v>200</v>
       </c>
-      <c r="AP2" s="4">
+      <c r="AQ2" s="4">
         <v>50</v>
       </c>
-      <c r="AQ2" s="4">
+      <c r="AR2" s="4">
         <v>60</v>
       </c>
-      <c r="AR2" s="5">
+      <c r="AS2" s="5">
         <v>0.76980000000000004</v>
       </c>
-      <c r="AS2">
+      <c r="AT2">
         <v>0.97260000000000002</v>
       </c>
-      <c r="AT2">
+      <c r="AU2">
         <v>0.59550000000000003</v>
       </c>
-      <c r="AU2" s="4">
+      <c r="AV2" s="4">
         <v>33</v>
       </c>
-      <c r="AV2" s="4">
+      <c r="AW2" s="4">
         <v>45</v>
       </c>
-      <c r="AW2" s="4">
+      <c r="AX2" s="4">
         <v>66</v>
       </c>
-      <c r="AX2" s="1">
+      <c r="AY2" s="1">
         <v>0.46</v>
       </c>
-      <c r="AY2" s="1">
+      <c r="AZ2" s="1">
         <f>1.25*0.46</f>
         <v>0.57500000000000007</v>
       </c>
-      <c r="AZ2" s="1">
+      <c r="BA2" s="1">
         <f>1.75 * 0.46</f>
         <v>0.80500000000000005</v>
       </c>
-      <c r="BA2" s="5">
+      <c r="BB2" s="5">
         <v>0.624</v>
       </c>
-      <c r="BB2" s="5">
+      <c r="BC2" s="5">
         <v>0.48599999999999999</v>
       </c>
-      <c r="BC2" s="1">
+      <c r="BD2" s="1">
         <v>200</v>
       </c>
-      <c r="BD2" s="1">
+      <c r="BE2" s="1">
         <v>0.79</v>
       </c>
-      <c r="BE2" s="1">
+      <c r="BF2" s="1">
         <f>(180+30+25)/60</f>
         <v>3.9166666666666665</v>
       </c>
-      <c r="BF2" s="1">
-        <f>3/BE2*125</f>
+      <c r="BG2" s="1">
+        <f>3/BF2*125</f>
         <v>95.744680851063833</v>
       </c>
-      <c r="BG2" s="1">
+      <c r="BH2" s="1">
         <f>65+32+3*2*(2*10+3*170)/15+25+45</f>
         <v>379</v>
       </c>
-      <c r="BH2" s="1">
+      <c r="BI2" s="1">
         <v>0.9</v>
       </c>
-      <c r="BI2" s="1">
+      <c r="BJ2" s="1">
         <v>1.5</v>
       </c>
-      <c r="BJ2" s="1">
+      <c r="BK2" s="1">
         <v>0.35</v>
       </c>
-      <c r="BK2" s="4">
+      <c r="BL2" s="4">
         <v>14</v>
       </c>
-      <c r="BL2">
+      <c r="BM2">
         <v>4.7</v>
       </c>
-      <c r="BM2">
+      <c r="BN2">
         <v>30</v>
       </c>
-      <c r="BN2" s="5">
+      <c r="BO2" s="5">
         <v>1.15E-2</v>
       </c>
-      <c r="BO2" s="1">
+      <c r="BP2" s="1">
         <v>263</v>
       </c>
-      <c r="BP2" s="1">
+      <c r="BQ2" s="1">
         <v>0.77</v>
       </c>
-      <c r="BQ2" s="4">
+      <c r="BR2" s="4">
         <v>105</v>
       </c>
-      <c r="BR2" s="4">
+      <c r="BS2" s="4">
         <v>80</v>
       </c>
-      <c r="BS2" s="4">
+      <c r="BT2" s="4">
         <v>28</v>
       </c>
-      <c r="BT2" s="4">
+      <c r="BU2" s="4">
         <v>43</v>
-      </c>
-      <c r="BU2" s="3">
-        <v>3</v>
       </c>
       <c r="BV2" s="3">
         <v>3</v>
       </c>
       <c r="BW2" s="3">
+        <v>3</v>
+      </c>
+      <c r="BX2" s="3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="BX2" s="3">
+      <c r="BY2" s="3">
         <v>5</v>
       </c>
-      <c r="BY2" s="4">
+      <c r="BZ2" s="4">
         <v>30</v>
       </c>
-      <c r="BZ2" s="1">
+      <c r="CA2" s="1">
         <v>0.01</v>
       </c>
-      <c r="CA2" s="1">
+      <c r="CB2" s="1">
         <v>264</v>
       </c>
-      <c r="CB2" s="1">
+      <c r="CC2" s="1">
         <v>0.77</v>
       </c>
-      <c r="CC2">
+      <c r="CD2">
         <v>45</v>
       </c>
-      <c r="CD2">
+      <c r="CE2">
         <v>0.72</v>
       </c>
-      <c r="CE2">
+      <c r="CF2">
         <v>4000</v>
       </c>
-      <c r="CF2">
+      <c r="CG2">
         <v>2000</v>
       </c>
-      <c r="CG2" s="1">
+      <c r="CH2" s="1">
         <v>360</v>
       </c>
-      <c r="CH2" s="1">
+      <c r="CI2" s="1">
         <v>0.8</v>
       </c>
-      <c r="CI2">
+      <c r="CJ2">
         <v>2900</v>
       </c>
-      <c r="CJ2">
+      <c r="CK2">
         <v>1550</v>
       </c>
-      <c r="CK2" s="1">
+      <c r="CL2" s="1">
         <v>248</v>
       </c>
-      <c r="CL2">
+      <c r="CM2">
         <v>0.75</v>
       </c>
-      <c r="CM2">
+      <c r="CN2">
         <v>21</v>
       </c>
-      <c r="CN2">
+      <c r="CO2">
         <v>30</v>
       </c>
-      <c r="CO2">
+      <c r="CP2">
         <v>1.5</v>
       </c>
-      <c r="CP2">
+      <c r="CQ2">
         <v>2.5</v>
       </c>
-      <c r="CQ2">
+      <c r="CR2">
         <v>4.5</v>
       </c>
-      <c r="CR2" s="3">
+      <c r="CS2" s="3">
         <v>6</v>
       </c>
-      <c r="CS2" s="1">
+      <c r="CT2" s="1">
         <v>204</v>
       </c>
-      <c r="CT2" s="1">
+      <c r="CU2" s="1">
         <v>0.89</v>
       </c>
-      <c r="CU2" s="4">
-        <f>2*CX2</f>
+      <c r="CV2" s="4">
+        <f>2*CY2</f>
         <v>52024.5</v>
       </c>
-      <c r="CV2" s="1">
+      <c r="CW2" s="1">
         <v>172</v>
       </c>
-      <c r="CW2" s="1">
+      <c r="CX2" s="1">
         <v>0.9</v>
       </c>
-      <c r="CX2" s="4">
+      <c r="CY2" s="4">
         <f>0.99*26275</f>
         <v>26012.25</v>
       </c>
-      <c r="CY2" s="1">
+      <c r="CZ2" s="1">
         <f>(180+17.5+17.5)/60</f>
         <v>3.5833333333333335</v>
       </c>
-      <c r="CZ2" s="1">
-        <f>3/CY2*100</f>
+      <c r="DA2" s="1">
+        <f>3/CZ2*100</f>
         <v>83.720930232558132</v>
       </c>
-      <c r="DA2" s="1">
+      <c r="DB2" s="1">
         <f>65+32+5*2*(2*10+3*170)/15+25+45</f>
         <v>520.33333333333326</v>
       </c>
-      <c r="DB2" s="1">
+      <c r="DC2" s="1">
         <v>1.5</v>
       </c>
-      <c r="DC2" s="1">
+      <c r="DD2" s="1">
         <f>0.35 + 0.12</f>
         <v>0.47</v>
       </c>
-      <c r="DD2" s="1">
-        <v>275</v>
-      </c>
       <c r="DE2" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="DF2" s="1">
         <f>145+200+383</f>
         <v>728</v>
+      </c>
+      <c r="DF2" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="DG2" s="1">
+        <v>275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
build: support cruised stands
</commit_message>
<xml_diff>
--- a/UnitTests/financial scenarios.xlsx
+++ b/UnitTests/financial scenarios.xlsx
@@ -1,34 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\westjoh\source\repos\SEEM\UnitTests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\westjoh\PhD\SEEM\UnitTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6075FE-5E8B-40A6-9EA2-591EC4340312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16188" windowHeight="7572"/>
+    <workbookView xWindow="1956" yWindow="1032" windowWidth="17280" windowHeight="11028" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameterization" sheetId="1" r:id="rId1"/>
     <sheet name="tracking list" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'tracking list'!$A$1:$C$113</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'tracking list'!$A$1:$C$116</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="139">
   <si>
     <t>name</t>
   </si>
@@ -436,12 +448,21 @@
   </si>
   <si>
     <t>thpl</t>
+  </si>
+  <si>
+    <t>alru2Spond</t>
+  </si>
+  <si>
+    <t>alru3Spond</t>
+  </si>
+  <si>
+    <t>alru4Spond</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
@@ -498,14 +519,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -791,23 +811,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DI4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:DL4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="15" max="24" width="8.88671875" customWidth="1"/>
-    <col min="108" max="113" width="8.88671875" customWidth="1"/>
+    <col min="18" max="27" width="8.88671875" customWidth="1"/>
+    <col min="111" max="116" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:113" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -827,328 +847,337 @@
         <v>9</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="R1" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="S1" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="W1" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="V1" s="10" t="s">
+      <c r="Y1" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AU1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AV1" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="BA1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AY1" s="2" t="s">
+      <c r="BB1" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="BC1" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="BA1" s="2" t="s">
+      <c r="BD1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="BB1" s="2" t="s">
+      <c r="BE1" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="BC1" s="2" t="s">
+      <c r="BF1" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="BD1" s="2" t="s">
+      <c r="BG1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="BE1" s="2" t="s">
+      <c r="BH1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="BF1" s="2" t="s">
+      <c r="BI1" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="BG1" s="2" t="s">
+      <c r="BJ1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="BH1" s="2" t="s">
+      <c r="BK1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="BI1" s="2" t="s">
+      <c r="BL1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="BJ1" s="2" t="s">
+      <c r="BM1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="BK1" s="2" t="s">
+      <c r="BN1" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="BL1" s="2" t="s">
+      <c r="BO1" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="BM1" s="2" t="s">
+      <c r="BP1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="BN1" s="2" t="s">
+      <c r="BQ1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="BO1" s="2" t="s">
+      <c r="BR1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="BP1" s="2" t="s">
+      <c r="BS1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="BQ1" s="2" t="s">
+      <c r="BT1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="BR1" s="2" t="s">
+      <c r="BU1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="BS1" s="11" t="s">
+      <c r="BV1" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="BT1" s="11" t="s">
+      <c r="BW1" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="BU1" s="2" t="s">
+      <c r="BX1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="BV1" s="2" t="s">
+      <c r="BY1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="BW1" s="2" t="s">
+      <c r="BZ1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="BX1" s="2" t="s">
+      <c r="CA1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="BY1" s="10" t="s">
+      <c r="CB1" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="BZ1" s="10" t="s">
+      <c r="CC1" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="CA1" s="2" t="s">
+      <c r="CD1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="CB1" s="2" t="s">
+      <c r="CE1" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="CC1" s="2" t="s">
+      <c r="CF1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="CD1" s="2" t="s">
+      <c r="CG1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="CE1" s="2" t="s">
+      <c r="CH1" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="CF1" s="2" t="s">
+      <c r="CI1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="CG1" s="2" t="s">
+      <c r="CJ1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="CH1" s="2" t="s">
+      <c r="CK1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="CI1" s="2" t="s">
+      <c r="CL1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="CJ1" s="2" t="s">
+      <c r="CM1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="CK1" s="2" t="s">
+      <c r="CN1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="CL1" s="2" t="s">
+      <c r="CO1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="CM1" s="2" t="s">
+      <c r="CP1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="CN1" s="2" t="s">
+      <c r="CQ1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="CO1" s="2" t="s">
+      <c r="CR1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="CP1" s="2" t="s">
+      <c r="CS1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="CQ1" s="2" t="s">
+      <c r="CT1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="CR1" s="2" t="s">
+      <c r="CU1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="CS1" s="2" t="s">
+      <c r="CV1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="CT1" s="2" t="s">
+      <c r="CW1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="CU1" s="2" t="s">
+      <c r="CX1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="CV1" s="2" t="s">
+      <c r="CY1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="CW1" s="2" t="s">
+      <c r="CZ1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="CX1" s="2" t="s">
+      <c r="DA1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="CY1" s="2" t="s">
+      <c r="DB1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="CZ1" s="2" t="s">
+      <c r="DC1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="DA1" s="2" t="s">
+      <c r="DD1" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="DB1" s="2" t="s">
+      <c r="DE1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="DC1" s="2" t="s">
+      <c r="DF1" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="DD1" s="2" t="s">
+      <c r="DG1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="DE1" s="2" t="s">
+      <c r="DH1" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="DF1" s="2" t="s">
+      <c r="DI1" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="DG1" s="2" t="s">
+      <c r="DJ1" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="DH1" s="2" t="s">
+      <c r="DK1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="DI1" s="2" t="s">
+      <c r="DL1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:113" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>133</v>
       </c>
@@ -1168,343 +1197,352 @@
         <v>1238</v>
       </c>
       <c r="G2">
+        <v>781</v>
+      </c>
+      <c r="H2">
+        <v>680</v>
+      </c>
+      <c r="I2">
+        <v>420</v>
+      </c>
+      <c r="J2">
         <v>531</v>
       </c>
-      <c r="H2">
+      <c r="K2">
         <v>525</v>
       </c>
-      <c r="I2">
+      <c r="L2">
         <v>454</v>
       </c>
-      <c r="J2" s="1">
+      <c r="M2" s="1">
         <v>0</v>
       </c>
-      <c r="K2">
+      <c r="N2">
         <v>37.71</v>
       </c>
-      <c r="L2">
+      <c r="O2">
         <v>4.1322000000000001</v>
       </c>
-      <c r="M2">
+      <c r="P2">
         <f>2*10+3*170</f>
         <v>530</v>
       </c>
-      <c r="N2">
+      <c r="Q2">
         <v>15</v>
       </c>
-      <c r="O2" s="4">
+      <c r="R2" s="4">
         <v>95</v>
       </c>
-      <c r="P2" s="4">
+      <c r="S2" s="4">
         <v>70</v>
       </c>
-      <c r="Q2" s="4">
+      <c r="T2" s="4">
         <v>28</v>
       </c>
-      <c r="R2" s="4">
+      <c r="U2" s="4">
         <v>43</v>
       </c>
-      <c r="S2" s="4">
+      <c r="V2" s="4">
         <v>6</v>
       </c>
-      <c r="T2" s="3">
+      <c r="W2" s="3">
         <v>1.9</v>
       </c>
-      <c r="U2" s="4">
+      <c r="X2" s="4">
         <v>45</v>
       </c>
-      <c r="V2" s="5">
+      <c r="Y2" s="5">
         <v>1.15E-2</v>
       </c>
-      <c r="W2" s="1">
+      <c r="Z2" s="1">
         <v>225</v>
       </c>
-      <c r="X2" s="1">
+      <c r="AA2" s="1">
         <v>0.77</v>
       </c>
-      <c r="Y2" s="3">
+      <c r="AB2" s="3">
         <v>51</v>
       </c>
-      <c r="Z2" s="3">
+      <c r="AC2" s="3">
         <v>54</v>
       </c>
-      <c r="AA2" s="4">
+      <c r="AD2" s="4">
         <v>30</v>
       </c>
-      <c r="AB2" s="1">
+      <c r="AE2" s="1">
         <v>1</v>
       </c>
-      <c r="AC2" s="1">
+      <c r="AF2" s="1">
         <v>80</v>
       </c>
-      <c r="AD2" s="1">
+      <c r="AG2" s="1">
         <v>0.75</v>
       </c>
-      <c r="AE2" s="1">
+      <c r="AH2" s="1">
         <v>2.17</v>
       </c>
-      <c r="AF2" s="1">
+      <c r="AI2" s="1">
         <v>0.25</v>
       </c>
-      <c r="AG2" s="4">
+      <c r="AJ2" s="4">
         <v>65</v>
       </c>
-      <c r="AH2" s="4">
+      <c r="AK2" s="4">
         <v>105</v>
       </c>
-      <c r="AI2" s="1">
+      <c r="AL2" s="1">
         <v>149.5</v>
       </c>
-      <c r="AJ2" s="1">
+      <c r="AM2" s="1">
         <v>0.5</v>
       </c>
-      <c r="AK2" s="4">
+      <c r="AN2" s="4">
         <v>50</v>
       </c>
-      <c r="AL2" s="5">
+      <c r="AO2" s="5">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="AM2" s="4">
+      <c r="AP2" s="4">
         <f>0.99*28990</f>
         <v>28700.1</v>
       </c>
-      <c r="AN2" s="4">
+      <c r="AQ2" s="4">
         <f>23700 + 1900 + 0.5 * 2 * 2600</f>
         <v>28200</v>
       </c>
-      <c r="AO2" s="4">
+      <c r="AR2" s="4">
         <v>20000</v>
       </c>
-      <c r="AP2" s="4">
+      <c r="AS2" s="4">
         <v>200</v>
       </c>
-      <c r="AQ2" s="4">
+      <c r="AT2" s="4">
         <v>50</v>
       </c>
-      <c r="AR2" s="4">
+      <c r="AU2" s="4">
         <v>60</v>
       </c>
-      <c r="AS2" s="5">
+      <c r="AV2" s="5">
         <v>0.76980000000000004</v>
       </c>
-      <c r="AT2">
+      <c r="AW2">
         <v>0.97260000000000002</v>
       </c>
-      <c r="AU2">
+      <c r="AX2">
         <v>0.59550000000000003</v>
       </c>
-      <c r="AV2" s="4">
+      <c r="AY2" s="4">
         <v>33</v>
       </c>
-      <c r="AW2" s="4">
+      <c r="AZ2" s="4">
         <v>45</v>
       </c>
-      <c r="AX2" s="4">
+      <c r="BA2" s="4">
         <v>66</v>
       </c>
-      <c r="AY2" s="1">
+      <c r="BB2" s="1">
         <v>0.46</v>
       </c>
-      <c r="AZ2" s="1">
+      <c r="BC2" s="1">
         <f>1.25*0.46</f>
         <v>0.57500000000000007</v>
       </c>
-      <c r="BA2" s="1">
+      <c r="BD2" s="1">
         <f>1.75 * 0.46</f>
         <v>0.80500000000000005</v>
       </c>
-      <c r="BB2" s="5">
+      <c r="BE2" s="5">
         <v>0.624</v>
       </c>
-      <c r="BC2" s="5">
+      <c r="BF2" s="5">
         <v>0.48599999999999999</v>
       </c>
-      <c r="BD2" s="1">
+      <c r="BG2" s="1">
         <v>200</v>
       </c>
-      <c r="BE2" s="1">
+      <c r="BH2" s="1">
         <v>0.79</v>
       </c>
-      <c r="BF2" s="4">
+      <c r="BI2" s="4">
         <v>350</v>
       </c>
-      <c r="BG2" s="1">
+      <c r="BJ2" s="1">
         <f>(180+30+25)/60</f>
         <v>3.9166666666666665</v>
       </c>
-      <c r="BH2" s="1">
-        <f>3/BG2*125</f>
+      <c r="BK2" s="1">
+        <f>3/BJ2*125</f>
         <v>95.744680851063833</v>
       </c>
-      <c r="BI2" s="1">
+      <c r="BL2" s="1">
         <f>65+32+3*2*(2*10+3*170)/15+25+45</f>
         <v>379</v>
       </c>
-      <c r="BJ2" s="1">
+      <c r="BM2" s="1">
         <v>0.9</v>
       </c>
-      <c r="BK2" s="1">
+      <c r="BN2" s="1">
         <v>1.5</v>
       </c>
-      <c r="BL2" s="1">
+      <c r="BO2" s="1">
         <v>0.35</v>
       </c>
-      <c r="BM2" s="4">
+      <c r="BP2" s="4">
         <v>14</v>
       </c>
-      <c r="BN2">
+      <c r="BQ2">
         <v>4.7</v>
       </c>
-      <c r="BO2">
+      <c r="BR2">
         <v>30</v>
       </c>
-      <c r="BP2" s="5">
+      <c r="BS2" s="5">
         <v>1.15E-2</v>
       </c>
-      <c r="BQ2" s="1">
+      <c r="BT2" s="1">
         <v>263</v>
       </c>
-      <c r="BR2" s="1">
+      <c r="BU2" s="1">
         <v>0.77</v>
       </c>
-      <c r="BS2" s="4">
+      <c r="BV2" s="4">
         <v>105</v>
       </c>
-      <c r="BT2" s="4">
+      <c r="BW2" s="4">
         <v>80</v>
       </c>
-      <c r="BU2" s="4">
+      <c r="BX2" s="4">
         <v>28</v>
       </c>
-      <c r="BV2" s="4">
+      <c r="BY2" s="4">
         <v>43</v>
       </c>
-      <c r="BW2" s="3">
+      <c r="BZ2" s="3">
         <v>3</v>
       </c>
-      <c r="BX2" s="3">
+      <c r="CA2" s="3">
         <v>3</v>
       </c>
-      <c r="BY2" s="3">
+      <c r="CB2" s="3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="BZ2" s="3">
+      <c r="CC2" s="3">
         <v>5</v>
       </c>
-      <c r="CA2" s="4">
+      <c r="CD2" s="4">
         <v>30</v>
       </c>
-      <c r="CB2" s="1">
+      <c r="CE2" s="1">
         <v>0.01</v>
       </c>
-      <c r="CC2" s="1">
+      <c r="CF2" s="1">
         <v>264</v>
       </c>
-      <c r="CD2" s="1">
+      <c r="CG2" s="1">
         <v>0.77</v>
       </c>
-      <c r="CE2" s="1">
+      <c r="CH2" s="1">
         <v>71.5</v>
       </c>
-      <c r="CF2">
+      <c r="CI2">
         <v>45</v>
       </c>
-      <c r="CG2">
+      <c r="CJ2">
         <v>0.72</v>
       </c>
-      <c r="CH2">
+      <c r="CK2">
         <v>4000</v>
       </c>
-      <c r="CI2">
+      <c r="CL2">
         <v>2000</v>
       </c>
-      <c r="CJ2" s="1">
+      <c r="CM2" s="1">
         <v>360</v>
       </c>
-      <c r="CK2" s="1">
+      <c r="CN2" s="1">
         <v>0.8</v>
       </c>
-      <c r="CL2">
+      <c r="CO2">
         <v>2900</v>
       </c>
-      <c r="CM2">
+      <c r="CP2">
         <v>1550</v>
       </c>
-      <c r="CN2" s="1">
+      <c r="CQ2" s="1">
         <v>248</v>
       </c>
-      <c r="CO2">
+      <c r="CR2">
         <v>0.75</v>
       </c>
-      <c r="CP2">
+      <c r="CS2">
         <v>21</v>
       </c>
-      <c r="CQ2">
+      <c r="CT2">
         <v>30</v>
       </c>
-      <c r="CR2">
+      <c r="CU2">
         <v>1.5</v>
       </c>
-      <c r="CS2">
+      <c r="CV2">
         <v>2.5</v>
       </c>
-      <c r="CT2">
+      <c r="CW2">
         <v>4.5</v>
       </c>
-      <c r="CU2" s="3">
+      <c r="CX2" s="3">
         <v>6</v>
       </c>
-      <c r="CV2" s="1">
+      <c r="CY2" s="1">
         <v>204</v>
       </c>
-      <c r="CW2" s="1">
+      <c r="CZ2" s="1">
         <v>0.89</v>
       </c>
-      <c r="CX2" s="4">
-        <f>2*DA2</f>
+      <c r="DA2" s="4">
+        <f>2*DD2</f>
         <v>52024.5</v>
       </c>
-      <c r="CY2" s="1">
+      <c r="DB2" s="1">
         <v>172</v>
       </c>
-      <c r="CZ2" s="1">
+      <c r="DC2" s="1">
         <v>0.9</v>
       </c>
-      <c r="DA2" s="4">
+      <c r="DD2" s="4">
         <f>0.99*26275</f>
         <v>26012.25</v>
       </c>
-      <c r="DB2" s="1">
+      <c r="DE2" s="1">
         <f>(180+17.5+17.5)/60</f>
         <v>3.5833333333333335</v>
       </c>
-      <c r="DC2" s="1">
-        <f>3/DB2*100</f>
+      <c r="DF2" s="1">
+        <f>3/DE2*100</f>
         <v>83.720930232558132</v>
       </c>
-      <c r="DD2" s="1">
+      <c r="DG2" s="1">
         <f>65+32+5*2*(2*10+3*170)/15+25+45</f>
         <v>520.33333333333326</v>
       </c>
-      <c r="DE2" s="1">
+      <c r="DH2" s="1">
         <v>1.5</v>
       </c>
-      <c r="DF2" s="1">
+      <c r="DI2" s="1">
         <f>0.35 + 0.12</f>
         <v>0.47</v>
       </c>
-      <c r="DG2" s="1">
+      <c r="DJ2" s="1">
         <f>145+200+383</f>
         <v>728</v>
       </c>
-      <c r="DH2" s="1">
+      <c r="DK2" s="1">
         <v>0.5</v>
       </c>
-      <c r="DI2" s="1">
+      <c r="DL2" s="1">
         <v>275</v>
       </c>
     </row>
-    <row r="3" spans="1:113" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>135</v>
       </c>
@@ -1524,343 +1562,352 @@
         <v>1238</v>
       </c>
       <c r="G3">
+        <v>781</v>
+      </c>
+      <c r="H3">
+        <v>680</v>
+      </c>
+      <c r="I3">
+        <v>420</v>
+      </c>
+      <c r="J3">
         <v>531</v>
       </c>
-      <c r="H3">
+      <c r="K3">
         <v>525</v>
       </c>
-      <c r="I3">
+      <c r="L3">
         <v>454</v>
       </c>
-      <c r="J3" s="1">
+      <c r="M3" s="1">
         <v>0</v>
       </c>
-      <c r="K3">
+      <c r="N3">
         <v>37.71</v>
       </c>
-      <c r="L3">
+      <c r="O3">
         <v>4.1322000000000001</v>
       </c>
-      <c r="M3">
+      <c r="P3">
         <f>2*10+3*170</f>
         <v>530</v>
       </c>
-      <c r="N3">
+      <c r="Q3">
         <v>15</v>
       </c>
-      <c r="O3" s="4">
+      <c r="R3" s="4">
         <v>76</v>
       </c>
-      <c r="P3" s="4">
+      <c r="S3" s="4">
         <v>58</v>
       </c>
-      <c r="Q3" s="4">
+      <c r="T3" s="4">
         <v>28</v>
       </c>
-      <c r="R3" s="4">
+      <c r="U3" s="4">
         <v>43</v>
       </c>
-      <c r="S3" s="4">
+      <c r="V3" s="4">
         <v>6</v>
       </c>
-      <c r="T3" s="3">
+      <c r="W3" s="3">
         <v>1.9</v>
       </c>
-      <c r="U3" s="4">
+      <c r="X3" s="4">
         <v>45</v>
       </c>
-      <c r="V3" s="5">
+      <c r="Y3" s="5">
         <v>1.15E-2</v>
       </c>
-      <c r="W3" s="1">
+      <c r="Z3" s="1">
         <v>225</v>
       </c>
-      <c r="X3" s="1">
+      <c r="AA3" s="1">
         <v>0.77</v>
       </c>
-      <c r="Y3" s="3">
+      <c r="AB3" s="3">
         <v>51</v>
       </c>
-      <c r="Z3" s="3">
+      <c r="AC3" s="3">
         <v>54</v>
       </c>
-      <c r="AA3" s="4">
+      <c r="AD3" s="4">
         <v>30</v>
       </c>
-      <c r="AB3" s="1">
+      <c r="AE3" s="1">
         <v>1</v>
       </c>
-      <c r="AC3" s="1">
+      <c r="AF3" s="1">
         <v>80</v>
       </c>
-      <c r="AD3" s="1">
+      <c r="AG3" s="1">
         <v>0.75</v>
       </c>
-      <c r="AE3" s="1">
+      <c r="AH3" s="1">
         <v>2.17</v>
       </c>
-      <c r="AF3" s="1">
+      <c r="AI3" s="1">
         <v>0.25</v>
       </c>
-      <c r="AG3" s="4">
+      <c r="AJ3" s="4">
         <v>65</v>
       </c>
-      <c r="AH3" s="4">
+      <c r="AK3" s="4">
         <v>105</v>
       </c>
-      <c r="AI3" s="1">
+      <c r="AL3" s="1">
         <v>149.5</v>
       </c>
-      <c r="AJ3" s="1">
+      <c r="AM3" s="1">
         <v>0.5</v>
       </c>
-      <c r="AK3" s="4">
+      <c r="AN3" s="4">
         <v>50</v>
       </c>
-      <c r="AL3" s="5">
+      <c r="AO3" s="5">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="AM3" s="4">
+      <c r="AP3" s="4">
         <f>0.99*28990</f>
         <v>28700.1</v>
       </c>
-      <c r="AN3" s="4">
+      <c r="AQ3" s="4">
         <f>23700 + 1900 + 0.5 * 2 * 2600</f>
         <v>28200</v>
       </c>
-      <c r="AO3" s="4">
+      <c r="AR3" s="4">
         <v>20000</v>
       </c>
-      <c r="AP3" s="4">
+      <c r="AS3" s="4">
         <v>200</v>
       </c>
-      <c r="AQ3" s="4">
+      <c r="AT3" s="4">
         <v>50</v>
       </c>
-      <c r="AR3" s="4">
+      <c r="AU3" s="4">
         <v>60</v>
       </c>
-      <c r="AS3" s="5">
+      <c r="AV3" s="5">
         <v>0.76980000000000004</v>
       </c>
-      <c r="AT3">
+      <c r="AW3">
         <v>0.97260000000000002</v>
       </c>
-      <c r="AU3">
+      <c r="AX3">
         <v>0.59550000000000003</v>
       </c>
-      <c r="AV3" s="4">
+      <c r="AY3" s="4">
         <v>33</v>
       </c>
-      <c r="AW3" s="4">
+      <c r="AZ3" s="4">
         <v>45</v>
       </c>
-      <c r="AX3" s="4">
+      <c r="BA3" s="4">
         <v>66</v>
       </c>
-      <c r="AY3" s="1">
+      <c r="BB3" s="1">
         <v>0.46</v>
       </c>
-      <c r="AZ3" s="1">
+      <c r="BC3" s="1">
         <f>1.25*0.46</f>
         <v>0.57500000000000007</v>
       </c>
-      <c r="BA3" s="1">
+      <c r="BD3" s="1">
         <f>1.75 * 0.46</f>
         <v>0.80500000000000005</v>
       </c>
-      <c r="BB3" s="5">
+      <c r="BE3" s="5">
         <v>0.624</v>
       </c>
-      <c r="BC3" s="5">
+      <c r="BF3" s="5">
         <v>0.48599999999999999</v>
       </c>
-      <c r="BD3" s="1">
+      <c r="BG3" s="1">
         <v>200</v>
       </c>
-      <c r="BE3" s="1">
+      <c r="BH3" s="1">
         <v>0.79</v>
       </c>
-      <c r="BF3" s="4">
+      <c r="BI3" s="4">
         <v>350</v>
       </c>
-      <c r="BG3" s="1">
+      <c r="BJ3" s="1">
         <f>(180+30+25)/60</f>
         <v>3.9166666666666665</v>
       </c>
-      <c r="BH3" s="1">
-        <f>3/BG3*125</f>
+      <c r="BK3" s="1">
+        <f>3/BJ3*125</f>
         <v>95.744680851063833</v>
       </c>
-      <c r="BI3" s="1">
+      <c r="BL3" s="1">
         <f>65+32+3*2*(2*10+3*170)/15+25+45</f>
         <v>379</v>
       </c>
-      <c r="BJ3" s="1">
+      <c r="BM3" s="1">
         <v>0.9</v>
       </c>
-      <c r="BK3" s="1">
+      <c r="BN3" s="1">
         <v>1.5</v>
       </c>
-      <c r="BL3" s="1">
+      <c r="BO3" s="1">
         <v>0.35</v>
       </c>
-      <c r="BM3" s="4">
+      <c r="BP3" s="4">
         <v>14</v>
       </c>
-      <c r="BN3">
+      <c r="BQ3">
         <v>4.7</v>
       </c>
-      <c r="BO3">
+      <c r="BR3">
         <v>30</v>
       </c>
-      <c r="BP3" s="5">
+      <c r="BS3" s="5">
         <v>1.15E-2</v>
       </c>
-      <c r="BQ3" s="1">
+      <c r="BT3" s="1">
         <v>263</v>
       </c>
-      <c r="BR3" s="1">
+      <c r="BU3" s="1">
         <v>0.77</v>
       </c>
-      <c r="BS3" s="4">
+      <c r="BV3" s="4">
         <v>85</v>
       </c>
-      <c r="BT3" s="4">
+      <c r="BW3" s="4">
         <v>67</v>
       </c>
-      <c r="BU3" s="4">
+      <c r="BX3" s="4">
         <v>28</v>
       </c>
-      <c r="BV3" s="4">
+      <c r="BY3" s="4">
         <v>43</v>
       </c>
-      <c r="BW3" s="3">
+      <c r="BZ3" s="3">
         <v>3</v>
       </c>
-      <c r="BX3" s="3">
+      <c r="CA3" s="3">
         <v>3</v>
       </c>
-      <c r="BY3" s="3">
+      <c r="CB3" s="3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="BZ3" s="3">
+      <c r="CC3" s="3">
         <v>5</v>
       </c>
-      <c r="CA3" s="4">
+      <c r="CD3" s="4">
         <v>30</v>
       </c>
-      <c r="CB3" s="1">
+      <c r="CE3" s="1">
         <v>0.01</v>
       </c>
-      <c r="CC3" s="1">
+      <c r="CF3" s="1">
         <v>264</v>
       </c>
-      <c r="CD3" s="1">
+      <c r="CG3" s="1">
         <v>0.77</v>
       </c>
-      <c r="CE3" s="1">
+      <c r="CH3" s="1">
         <v>71.5</v>
       </c>
-      <c r="CF3">
+      <c r="CI3">
         <v>45</v>
       </c>
-      <c r="CG3">
+      <c r="CJ3">
         <v>0.72</v>
       </c>
-      <c r="CH3">
+      <c r="CK3">
         <v>4000</v>
       </c>
-      <c r="CI3">
+      <c r="CL3">
         <v>2000</v>
       </c>
-      <c r="CJ3" s="1">
+      <c r="CM3" s="1">
         <v>360</v>
       </c>
-      <c r="CK3" s="1">
+      <c r="CN3" s="1">
         <v>0.8</v>
       </c>
-      <c r="CL3">
+      <c r="CO3">
         <v>2900</v>
       </c>
-      <c r="CM3">
+      <c r="CP3">
         <v>1550</v>
       </c>
-      <c r="CN3" s="1">
+      <c r="CQ3" s="1">
         <v>248</v>
       </c>
-      <c r="CO3">
+      <c r="CR3">
         <v>0.75</v>
       </c>
-      <c r="CP3">
+      <c r="CS3">
         <v>21</v>
       </c>
-      <c r="CQ3">
+      <c r="CT3">
         <v>30</v>
       </c>
-      <c r="CR3">
+      <c r="CU3">
         <v>1.5</v>
       </c>
-      <c r="CS3">
+      <c r="CV3">
         <v>2.5</v>
       </c>
-      <c r="CT3">
+      <c r="CW3">
         <v>4.5</v>
       </c>
-      <c r="CU3" s="3">
+      <c r="CX3" s="3">
         <v>6</v>
       </c>
-      <c r="CV3" s="1">
+      <c r="CY3" s="1">
         <v>204</v>
       </c>
-      <c r="CW3" s="1">
+      <c r="CZ3" s="1">
         <v>0.89</v>
       </c>
-      <c r="CX3" s="4">
-        <f>2*DA3</f>
+      <c r="DA3" s="4">
+        <f>2*DD3</f>
         <v>52024.5</v>
       </c>
-      <c r="CY3" s="1">
+      <c r="DB3" s="1">
         <v>172</v>
       </c>
-      <c r="CZ3" s="1">
+      <c r="DC3" s="1">
         <v>0.9</v>
       </c>
-      <c r="DA3" s="4">
+      <c r="DD3" s="4">
         <f>0.99*26275</f>
         <v>26012.25</v>
       </c>
-      <c r="DB3" s="1">
+      <c r="DE3" s="1">
         <f>(180+17.5+17.5)/60</f>
         <v>3.5833333333333335</v>
       </c>
-      <c r="DC3" s="1">
-        <f>3/DB3*100</f>
+      <c r="DF3" s="1">
+        <f>3/DE3*100</f>
         <v>83.720930232558132</v>
       </c>
-      <c r="DD3" s="1">
+      <c r="DG3" s="1">
         <f>65+32+5*2*(2*10+3*170)/15+25+45</f>
         <v>520.33333333333326</v>
       </c>
-      <c r="DE3" s="1">
+      <c r="DH3" s="1">
         <v>1.5</v>
       </c>
-      <c r="DF3" s="1">
+      <c r="DI3" s="1">
         <f>0.35 + 0.12</f>
         <v>0.47</v>
       </c>
-      <c r="DG3" s="1">
+      <c r="DJ3" s="1">
         <f>145+200+383</f>
         <v>728</v>
       </c>
-      <c r="DH3" s="1">
+      <c r="DK3" s="1">
         <v>0.5</v>
       </c>
-      <c r="DI3" s="1">
+      <c r="DL3" s="1">
         <v>275</v>
       </c>
     </row>
-    <row r="4" spans="1:113" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:116" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>134</v>
       </c>
@@ -1880,339 +1927,348 @@
         <v>1238</v>
       </c>
       <c r="G4">
+        <v>781</v>
+      </c>
+      <c r="H4">
+        <v>680</v>
+      </c>
+      <c r="I4">
+        <v>420</v>
+      </c>
+      <c r="J4">
         <v>531</v>
       </c>
-      <c r="H4">
+      <c r="K4">
         <v>525</v>
       </c>
-      <c r="I4">
+      <c r="L4">
         <v>454</v>
       </c>
-      <c r="J4" s="1">
+      <c r="M4" s="1">
         <v>0</v>
       </c>
-      <c r="K4">
+      <c r="N4">
         <v>37.71</v>
       </c>
-      <c r="L4">
+      <c r="O4">
         <v>4.1322000000000001</v>
       </c>
-      <c r="M4">
+      <c r="P4">
         <f>2*10+3*170</f>
         <v>530</v>
       </c>
-      <c r="N4">
+      <c r="Q4">
         <v>15</v>
       </c>
-      <c r="O4" s="4">
+      <c r="R4" s="4">
         <v>88</v>
       </c>
-      <c r="P4" s="4">
+      <c r="S4" s="4">
         <v>67</v>
       </c>
-      <c r="Q4" s="4">
+      <c r="T4" s="4">
         <v>28</v>
       </c>
-      <c r="R4" s="4">
+      <c r="U4" s="4">
         <v>43</v>
       </c>
-      <c r="S4" s="4">
+      <c r="V4" s="4">
         <v>6</v>
       </c>
-      <c r="T4" s="3">
+      <c r="W4" s="3">
         <v>1.9</v>
       </c>
-      <c r="U4" s="4">
+      <c r="X4" s="4">
         <v>45</v>
       </c>
-      <c r="V4" s="5">
+      <c r="Y4" s="5">
         <v>1.15E-2</v>
       </c>
-      <c r="W4" s="1">
+      <c r="Z4" s="1">
         <v>225</v>
       </c>
-      <c r="X4" s="1">
+      <c r="AA4" s="1">
         <v>0.77</v>
       </c>
-      <c r="Y4" s="3">
+      <c r="AB4" s="3">
         <v>51</v>
       </c>
-      <c r="Z4" s="3">
+      <c r="AC4" s="3">
         <v>54</v>
       </c>
-      <c r="AA4" s="4">
+      <c r="AD4" s="4">
         <v>30</v>
       </c>
-      <c r="AB4" s="1">
+      <c r="AE4" s="1">
         <v>1</v>
       </c>
-      <c r="AC4" s="1">
+      <c r="AF4" s="1">
         <v>80</v>
       </c>
-      <c r="AD4" s="1">
+      <c r="AG4" s="1">
         <v>0.75</v>
       </c>
-      <c r="AE4" s="1">
+      <c r="AH4" s="1">
         <v>2.17</v>
       </c>
-      <c r="AF4" s="1">
+      <c r="AI4" s="1">
         <v>0.25</v>
       </c>
-      <c r="AG4" s="4">
+      <c r="AJ4" s="4">
         <v>65</v>
       </c>
-      <c r="AH4" s="4">
+      <c r="AK4" s="4">
         <v>105</v>
       </c>
-      <c r="AI4" s="1">
+      <c r="AL4" s="1">
         <v>149.5</v>
       </c>
-      <c r="AJ4" s="1">
+      <c r="AM4" s="1">
         <v>0.5</v>
       </c>
-      <c r="AK4" s="4">
+      <c r="AN4" s="4">
         <v>50</v>
       </c>
-      <c r="AL4" s="5">
+      <c r="AO4" s="5">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="AM4" s="4">
+      <c r="AP4" s="4">
         <f>0.99*28990</f>
         <v>28700.1</v>
       </c>
-      <c r="AN4" s="4">
+      <c r="AQ4" s="4">
         <f>23700 + 1900 + 0.5 * 2 * 2600</f>
         <v>28200</v>
       </c>
-      <c r="AO4" s="4">
+      <c r="AR4" s="4">
         <v>20000</v>
       </c>
-      <c r="AP4" s="4">
+      <c r="AS4" s="4">
         <v>200</v>
       </c>
-      <c r="AQ4" s="4">
+      <c r="AT4" s="4">
         <v>50</v>
       </c>
-      <c r="AR4" s="4">
+      <c r="AU4" s="4">
         <v>60</v>
       </c>
-      <c r="AS4" s="5">
+      <c r="AV4" s="5">
         <v>0.76980000000000004</v>
       </c>
-      <c r="AT4">
+      <c r="AW4">
         <v>0.97260000000000002</v>
       </c>
-      <c r="AU4">
+      <c r="AX4">
         <v>0.59550000000000003</v>
       </c>
-      <c r="AV4" s="4">
+      <c r="AY4" s="4">
         <v>33</v>
       </c>
-      <c r="AW4" s="4">
+      <c r="AZ4" s="4">
         <v>45</v>
       </c>
-      <c r="AX4" s="4">
+      <c r="BA4" s="4">
         <v>66</v>
       </c>
-      <c r="AY4" s="1">
+      <c r="BB4" s="1">
         <v>0.46</v>
       </c>
-      <c r="AZ4" s="1">
+      <c r="BC4" s="1">
         <f>1.25*0.46</f>
         <v>0.57500000000000007</v>
       </c>
-      <c r="BA4" s="1">
+      <c r="BD4" s="1">
         <f>1.75 * 0.46</f>
         <v>0.80500000000000005</v>
       </c>
-      <c r="BB4" s="5">
+      <c r="BE4" s="5">
         <v>0.624</v>
       </c>
-      <c r="BC4" s="5">
+      <c r="BF4" s="5">
         <v>0.48599999999999999</v>
       </c>
-      <c r="BD4" s="1">
+      <c r="BG4" s="1">
         <v>200</v>
       </c>
-      <c r="BE4" s="1">
+      <c r="BH4" s="1">
         <v>0.79</v>
       </c>
-      <c r="BF4" s="4">
+      <c r="BI4" s="4">
         <v>350</v>
       </c>
-      <c r="BG4" s="1">
+      <c r="BJ4" s="1">
         <f>(180+30+25)/60</f>
         <v>3.9166666666666665</v>
       </c>
-      <c r="BH4" s="1">
-        <f>3/BG4*125</f>
+      <c r="BK4" s="1">
+        <f>3/BJ4*125</f>
         <v>95.744680851063833</v>
       </c>
-      <c r="BI4" s="1">
+      <c r="BL4" s="1">
         <f>65+32+3*2*(2*10+3*170)/15+25+45</f>
         <v>379</v>
       </c>
-      <c r="BJ4" s="1">
+      <c r="BM4" s="1">
         <v>0.9</v>
       </c>
-      <c r="BK4" s="1">
+      <c r="BN4" s="1">
         <v>1.5</v>
       </c>
-      <c r="BL4" s="1">
+      <c r="BO4" s="1">
         <v>0.35</v>
       </c>
-      <c r="BM4" s="4">
+      <c r="BP4" s="4">
         <v>14</v>
       </c>
-      <c r="BN4">
+      <c r="BQ4">
         <v>4.7</v>
       </c>
-      <c r="BO4">
+      <c r="BR4">
         <v>30</v>
       </c>
-      <c r="BP4" s="5">
+      <c r="BS4" s="5">
         <v>1.15E-2</v>
       </c>
-      <c r="BQ4" s="1">
+      <c r="BT4" s="1">
         <v>263</v>
       </c>
-      <c r="BR4" s="1">
+      <c r="BU4" s="1">
         <v>0.77</v>
       </c>
-      <c r="BS4" s="4">
+      <c r="BV4" s="4">
         <v>98</v>
       </c>
-      <c r="BT4" s="4">
+      <c r="BW4" s="4">
         <v>78</v>
       </c>
-      <c r="BU4" s="4">
+      <c r="BX4" s="4">
         <v>28</v>
       </c>
-      <c r="BV4" s="4">
+      <c r="BY4" s="4">
         <v>43</v>
       </c>
-      <c r="BW4" s="3">
+      <c r="BZ4" s="3">
         <v>3</v>
       </c>
-      <c r="BX4" s="3">
+      <c r="CA4" s="3">
         <v>3</v>
       </c>
-      <c r="BY4" s="3">
+      <c r="CB4" s="3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="BZ4" s="3">
+      <c r="CC4" s="3">
         <v>5</v>
       </c>
-      <c r="CA4" s="4">
+      <c r="CD4" s="4">
         <v>30</v>
       </c>
-      <c r="CB4" s="1">
+      <c r="CE4" s="1">
         <v>0.01</v>
       </c>
-      <c r="CC4" s="1">
+      <c r="CF4" s="1">
         <v>264</v>
       </c>
-      <c r="CD4" s="1">
+      <c r="CG4" s="1">
         <v>0.77</v>
       </c>
-      <c r="CE4" s="1">
+      <c r="CH4" s="1">
         <v>71.5</v>
       </c>
-      <c r="CF4">
+      <c r="CI4">
         <v>45</v>
       </c>
-      <c r="CG4">
+      <c r="CJ4">
         <v>0.72</v>
       </c>
-      <c r="CH4">
+      <c r="CK4">
         <v>4000</v>
       </c>
-      <c r="CI4">
+      <c r="CL4">
         <v>2000</v>
       </c>
-      <c r="CJ4" s="1">
+      <c r="CM4" s="1">
         <v>360</v>
       </c>
-      <c r="CK4" s="1">
+      <c r="CN4" s="1">
         <v>0.8</v>
       </c>
-      <c r="CL4">
+      <c r="CO4">
         <v>2900</v>
       </c>
-      <c r="CM4">
+      <c r="CP4">
         <v>1550</v>
       </c>
-      <c r="CN4" s="1">
+      <c r="CQ4" s="1">
         <v>248</v>
       </c>
-      <c r="CO4">
+      <c r="CR4">
         <v>0.75</v>
       </c>
-      <c r="CP4">
+      <c r="CS4">
         <v>21</v>
       </c>
-      <c r="CQ4">
+      <c r="CT4">
         <v>30</v>
       </c>
-      <c r="CR4">
+      <c r="CU4">
         <v>1.5</v>
       </c>
-      <c r="CS4">
+      <c r="CV4">
         <v>2.5</v>
       </c>
-      <c r="CT4">
+      <c r="CW4">
         <v>4.5</v>
       </c>
-      <c r="CU4" s="3">
+      <c r="CX4" s="3">
         <v>6</v>
       </c>
-      <c r="CV4" s="1">
+      <c r="CY4" s="1">
         <v>204</v>
       </c>
-      <c r="CW4" s="1">
+      <c r="CZ4" s="1">
         <v>0.89</v>
       </c>
-      <c r="CX4" s="4">
-        <f>2*DA4</f>
+      <c r="DA4" s="4">
+        <f>2*DD4</f>
         <v>52024.5</v>
       </c>
-      <c r="CY4" s="1">
+      <c r="DB4" s="1">
         <v>172</v>
       </c>
-      <c r="CZ4" s="1">
+      <c r="DC4" s="1">
         <v>0.9</v>
       </c>
-      <c r="DA4" s="4">
+      <c r="DD4" s="4">
         <f>0.99*26275</f>
         <v>26012.25</v>
       </c>
-      <c r="DB4" s="1">
+      <c r="DE4" s="1">
         <f>(180+17.5+17.5)/60</f>
         <v>3.5833333333333335</v>
       </c>
-      <c r="DC4" s="1">
-        <f>3/DB4*100</f>
+      <c r="DF4" s="1">
+        <f>3/DE4*100</f>
         <v>83.720930232558132</v>
       </c>
-      <c r="DD4" s="1">
+      <c r="DG4" s="1">
         <f>65+32+5*2*(2*10+3*170)/15+25+45</f>
         <v>520.33333333333326</v>
       </c>
-      <c r="DE4" s="1">
+      <c r="DH4" s="1">
         <v>1.5</v>
       </c>
-      <c r="DF4" s="1">
+      <c r="DI4" s="1">
         <f>0.35 + 0.12</f>
         <v>0.47</v>
       </c>
-      <c r="DG4" s="1">
+      <c r="DJ4" s="1">
         <f>145+200+383</f>
         <v>728</v>
       </c>
-      <c r="DH4" s="1">
+      <c r="DK4" s="1">
         <v>0.5</v>
       </c>
-      <c r="DI4" s="1">
+      <c r="DL4" s="1">
         <v>275</v>
       </c>
     </row>
@@ -2223,12 +2279,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F119"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F122"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2255,7 +2311,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -2268,12 +2324,12 @@
         <v>107</v>
       </c>
       <c r="F2">
-        <f>COUNTIFS(B2:B119,E2) - 1</f>
+        <f>COUNTIFS(B2:B122,E2) - 1</f>
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -2286,13 +2342,13 @@
         <v>109</v>
       </c>
       <c r="F3">
-        <f>COUNTIFS(B2:B119,E3)</f>
+        <f>COUNTIFS(B2:B122,E3)</f>
         <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>6</v>
+      <c r="A4" t="s">
+        <v>136</v>
       </c>
       <c r="B4" t="s">
         <v>108</v>
@@ -2304,13 +2360,13 @@
         <v>108</v>
       </c>
       <c r="F4">
-        <f>COUNTIFS(B2:B119,E4)</f>
-        <v>9</v>
+        <f>COUNTIFS(B2:B122,E4)</f>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>7</v>
+      <c r="A5" t="s">
+        <v>137</v>
       </c>
       <c r="B5" t="s">
         <v>108</v>
@@ -2323,12 +2379,12 @@
       </c>
       <c r="F5">
         <f>SUM(F2:F4)</f>
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
-        <v>8</v>
+      <c r="A6" t="s">
+        <v>138</v>
       </c>
       <c r="B6" t="s">
         <v>108</v>
@@ -2338,8 +2394,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>9</v>
+      <c r="A7" t="s">
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>108</v>
@@ -2349,8 +2405,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>10</v>
+      <c r="A8" t="s">
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>108</v>
@@ -2360,8 +2416,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>11</v>
+      <c r="A9" t="s">
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>108</v>
@@ -2371,8 +2427,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>12</v>
+      <c r="A10" t="s">
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>108</v>
@@ -2382,8 +2438,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>5</v>
+      <c r="A11" t="s">
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>108</v>
@@ -2393,338 +2449,338 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C14" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>17</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B15" t="s">
         <v>107</v>
       </c>
-      <c r="C12" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
+      <c r="C15" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>16</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B16" t="s">
         <v>107</v>
       </c>
-      <c r="C13" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+      <c r="C16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="B14" t="s">
-        <v>109</v>
-      </c>
-      <c r="C14" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
+      <c r="B17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>90</v>
       </c>
-      <c r="B15" t="s">
-        <v>109</v>
-      </c>
-      <c r="C15" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
+      <c r="B18" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="B16" t="s">
-        <v>109</v>
-      </c>
-      <c r="C16" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
+      <c r="B19" t="s">
+        <v>109</v>
+      </c>
+      <c r="C19" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>91</v>
       </c>
-      <c r="B17" t="s">
-        <v>109</v>
-      </c>
-      <c r="C17" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
+      <c r="B20" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>22</v>
       </c>
-      <c r="B18" t="s">
-        <v>109</v>
-      </c>
-      <c r="C18" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
+      <c r="B21" t="s">
+        <v>109</v>
+      </c>
+      <c r="C21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>24</v>
       </c>
-      <c r="B19" t="s">
-        <v>109</v>
-      </c>
-      <c r="C19" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
+      <c r="B22" t="s">
+        <v>109</v>
+      </c>
+      <c r="C22" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>112</v>
       </c>
-      <c r="B20" t="s">
-        <v>109</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="B23" t="s">
+        <v>109</v>
+      </c>
+      <c r="C23" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>114</v>
       </c>
-      <c r="B21" t="s">
-        <v>109</v>
-      </c>
-      <c r="C21" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
+      <c r="B24" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>117</v>
       </c>
-      <c r="B22" t="s">
-        <v>109</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="B25" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="6" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>104</v>
       </c>
-      <c r="B23" t="s">
-        <v>109</v>
-      </c>
-      <c r="C23" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="6" t="s">
+      <c r="B26" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>103</v>
       </c>
-      <c r="B24" t="s">
-        <v>109</v>
-      </c>
-      <c r="C24" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="6" t="s">
+      <c r="B27" t="s">
+        <v>109</v>
+      </c>
+      <c r="C27" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>20</v>
       </c>
-      <c r="B25" t="s">
-        <v>109</v>
-      </c>
-      <c r="C25" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="6" t="s">
+      <c r="B28" t="s">
+        <v>109</v>
+      </c>
+      <c r="C28" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>21</v>
       </c>
-      <c r="B26" t="s">
-        <v>109</v>
-      </c>
-      <c r="C26" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="6" t="s">
+      <c r="B29" t="s">
+        <v>109</v>
+      </c>
+      <c r="C29" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>23</v>
       </c>
-      <c r="B27" t="s">
-        <v>109</v>
-      </c>
-      <c r="C27" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="6" t="s">
+      <c r="B30" t="s">
+        <v>109</v>
+      </c>
+      <c r="C30" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>98</v>
       </c>
-      <c r="B28" t="s">
-        <v>109</v>
-      </c>
-      <c r="C28" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="6" t="s">
+      <c r="B31" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>99</v>
       </c>
-      <c r="B29" t="s">
-        <v>109</v>
-      </c>
-      <c r="C29" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="6" t="s">
+      <c r="B32" t="s">
+        <v>109</v>
+      </c>
+      <c r="C32" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>100</v>
       </c>
-      <c r="B30" t="s">
-        <v>109</v>
-      </c>
-      <c r="C30" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="6" t="s">
+      <c r="B33" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>101</v>
       </c>
-      <c r="B31" t="s">
-        <v>109</v>
-      </c>
-      <c r="C31" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="6" t="s">
+      <c r="B34" t="s">
+        <v>109</v>
+      </c>
+      <c r="C34" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>102</v>
       </c>
-      <c r="B32" t="s">
-        <v>109</v>
-      </c>
-      <c r="C32" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="6" t="s">
+      <c r="B35" t="s">
+        <v>109</v>
+      </c>
+      <c r="C35" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>73</v>
       </c>
-      <c r="B33" t="s">
-        <v>109</v>
-      </c>
-      <c r="C33" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="6" t="s">
+      <c r="B36" t="s">
+        <v>109</v>
+      </c>
+      <c r="C36" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>72</v>
       </c>
-      <c r="B34" t="s">
-        <v>109</v>
-      </c>
-      <c r="C34" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="6" t="s">
+      <c r="B37" t="s">
+        <v>109</v>
+      </c>
+      <c r="C37" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>87</v>
       </c>
-      <c r="B35" t="s">
-        <v>109</v>
-      </c>
-      <c r="C35" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="6" t="s">
+      <c r="B38" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>86</v>
       </c>
-      <c r="B36" t="s">
-        <v>109</v>
-      </c>
-      <c r="C36" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="6" t="s">
+      <c r="B39" t="s">
+        <v>109</v>
+      </c>
+      <c r="C39" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>49</v>
       </c>
-      <c r="B37" t="s">
-        <v>109</v>
-      </c>
-      <c r="C37" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="6" t="s">
+      <c r="B40" t="s">
+        <v>109</v>
+      </c>
+      <c r="C40" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>50</v>
       </c>
-      <c r="B38" t="s">
-        <v>109</v>
-      </c>
-      <c r="C38" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="6" t="s">
+      <c r="B41" t="s">
+        <v>109</v>
+      </c>
+      <c r="C41" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>51</v>
-      </c>
-      <c r="B39" t="s">
-        <v>109</v>
-      </c>
-      <c r="C39" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B40" t="s">
-        <v>109</v>
-      </c>
-      <c r="C40" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B41" t="s">
-        <v>109</v>
-      </c>
-      <c r="C41" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="B42" t="s">
         <v>109</v>
@@ -2735,7 +2791,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="B43" t="s">
         <v>109</v>
@@ -2745,8 +2801,8 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="6" t="s">
-        <v>69</v>
+      <c r="A44" t="s">
+        <v>53</v>
       </c>
       <c r="B44" t="s">
         <v>109</v>
@@ -2757,469 +2813,469 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B45" t="s">
+        <v>109</v>
+      </c>
+      <c r="C45" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>68</v>
+      </c>
+      <c r="B46" t="s">
+        <v>109</v>
+      </c>
+      <c r="C46" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>69</v>
+      </c>
+      <c r="B47" t="s">
+        <v>109</v>
+      </c>
+      <c r="C47" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>61</v>
       </c>
-      <c r="B45" t="s">
-        <v>109</v>
-      </c>
-      <c r="C45" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="6" t="s">
+      <c r="B48" t="s">
+        <v>109</v>
+      </c>
+      <c r="C48" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>62</v>
       </c>
-      <c r="B46" t="s">
-        <v>109</v>
-      </c>
-      <c r="C46" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="6" t="s">
+      <c r="B49" t="s">
+        <v>109</v>
+      </c>
+      <c r="C49" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>63</v>
       </c>
-      <c r="B47" t="s">
-        <v>109</v>
-      </c>
-      <c r="C47" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="6" t="s">
+      <c r="B50" t="s">
+        <v>109</v>
+      </c>
+      <c r="C50" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>64</v>
       </c>
-      <c r="B48" t="s">
-        <v>109</v>
-      </c>
-      <c r="C48" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="6" t="s">
+      <c r="B51" t="s">
+        <v>109</v>
+      </c>
+      <c r="C51" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>80</v>
       </c>
-      <c r="B49" t="s">
-        <v>109</v>
-      </c>
-      <c r="C49" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="6" t="s">
+      <c r="B52" t="s">
+        <v>109</v>
+      </c>
+      <c r="C52" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>81</v>
       </c>
-      <c r="B50" t="s">
-        <v>109</v>
-      </c>
-      <c r="C50" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="6" t="s">
+      <c r="B53" t="s">
+        <v>109</v>
+      </c>
+      <c r="C53" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>77</v>
       </c>
-      <c r="B51" t="s">
-        <v>109</v>
-      </c>
-      <c r="C51" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="6" t="s">
+      <c r="B54" t="s">
+        <v>109</v>
+      </c>
+      <c r="C54" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>76</v>
       </c>
-      <c r="B52" t="s">
-        <v>109</v>
-      </c>
-      <c r="C52" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="6" t="s">
+      <c r="B55" t="s">
+        <v>109</v>
+      </c>
+      <c r="C55" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>65</v>
       </c>
-      <c r="B53" t="s">
-        <v>109</v>
-      </c>
-      <c r="C53" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="6" t="s">
+      <c r="B56" t="s">
+        <v>109</v>
+      </c>
+      <c r="C56" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>66</v>
       </c>
-      <c r="B54" t="s">
-        <v>109</v>
-      </c>
-      <c r="C54" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" s="6" t="s">
+      <c r="B57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C57" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>79</v>
       </c>
-      <c r="B55" t="s">
-        <v>109</v>
-      </c>
-      <c r="C55" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="6" t="s">
+      <c r="B58" t="s">
+        <v>109</v>
+      </c>
+      <c r="C58" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>78</v>
       </c>
-      <c r="B56" t="s">
-        <v>109</v>
-      </c>
-      <c r="C56" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" s="6" t="s">
+      <c r="B59" t="s">
+        <v>109</v>
+      </c>
+      <c r="C59" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>67</v>
       </c>
-      <c r="B57" t="s">
-        <v>109</v>
-      </c>
-      <c r="C57" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" s="6" t="s">
+      <c r="B60" t="s">
+        <v>109</v>
+      </c>
+      <c r="C60" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
         <v>83</v>
       </c>
-      <c r="B58" t="s">
-        <v>109</v>
-      </c>
-      <c r="C58" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" s="6" t="s">
+      <c r="B61" t="s">
+        <v>109</v>
+      </c>
+      <c r="C61" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>92</v>
       </c>
-      <c r="B59" t="s">
-        <v>109</v>
-      </c>
-      <c r="C59" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" s="6" t="s">
+      <c r="B62" t="s">
+        <v>109</v>
+      </c>
+      <c r="C62" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
         <v>93</v>
       </c>
-      <c r="B60" t="s">
-        <v>109</v>
-      </c>
-      <c r="C60" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" s="6" t="s">
+      <c r="B63" t="s">
+        <v>109</v>
+      </c>
+      <c r="C63" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>94</v>
       </c>
-      <c r="B61" t="s">
-        <v>109</v>
-      </c>
-      <c r="C61" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" s="6" t="s">
+      <c r="B64" t="s">
+        <v>109</v>
+      </c>
+      <c r="C64" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
         <v>14</v>
       </c>
-      <c r="B62" t="s">
-        <v>109</v>
-      </c>
-      <c r="C62" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" s="6" t="s">
+      <c r="B65" t="s">
+        <v>109</v>
+      </c>
+      <c r="C65" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
         <v>13</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B66" t="s">
         <v>108</v>
       </c>
-      <c r="C63" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" s="6" t="s">
+      <c r="C66" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
         <v>126</v>
       </c>
-      <c r="B64" t="s">
-        <v>109</v>
-      </c>
-      <c r="C64" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" s="6" t="s">
+      <c r="B67" t="s">
+        <v>109</v>
+      </c>
+      <c r="C67" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
         <v>127</v>
       </c>
-      <c r="B65" t="s">
-        <v>109</v>
-      </c>
-      <c r="C65" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" s="6" t="s">
+      <c r="B68" t="s">
+        <v>109</v>
+      </c>
+      <c r="C68" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
         <v>25</v>
       </c>
-      <c r="B66" t="s">
-        <v>109</v>
-      </c>
-      <c r="C66" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" s="6" t="s">
+      <c r="B69" t="s">
+        <v>109</v>
+      </c>
+      <c r="C69" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
         <v>26</v>
       </c>
-      <c r="B67" t="s">
-        <v>109</v>
-      </c>
-      <c r="C67" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" s="6" t="s">
+      <c r="B70" t="s">
+        <v>109</v>
+      </c>
+      <c r="C70" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
         <v>27</v>
       </c>
-      <c r="B68" t="s">
-        <v>109</v>
-      </c>
-      <c r="C68" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" s="6" t="s">
+      <c r="B71" t="s">
+        <v>109</v>
+      </c>
+      <c r="C71" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
         <v>84</v>
       </c>
-      <c r="B69" t="s">
-        <v>109</v>
-      </c>
-      <c r="C69" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" s="6" t="s">
+      <c r="B72" t="s">
+        <v>109</v>
+      </c>
+      <c r="C72" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
         <v>75</v>
       </c>
-      <c r="B70" t="s">
-        <v>109</v>
-      </c>
-      <c r="C70" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71" s="6" t="s">
+      <c r="B73" t="s">
+        <v>109</v>
+      </c>
+      <c r="C73" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
         <v>74</v>
       </c>
-      <c r="B71" t="s">
-        <v>109</v>
-      </c>
-      <c r="C71" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72" s="6" t="s">
+      <c r="B74" t="s">
+        <v>109</v>
+      </c>
+      <c r="C74" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
         <v>89</v>
       </c>
-      <c r="B72" t="s">
-        <v>109</v>
-      </c>
-      <c r="C72" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" s="6" t="s">
+      <c r="B75" t="s">
+        <v>109</v>
+      </c>
+      <c r="C75" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
         <v>88</v>
       </c>
-      <c r="B73" t="s">
-        <v>109</v>
-      </c>
-      <c r="C73" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" s="6" t="s">
+      <c r="B76" t="s">
+        <v>109</v>
+      </c>
+      <c r="C76" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
         <v>54</v>
       </c>
-      <c r="B74" t="s">
-        <v>109</v>
-      </c>
-      <c r="C74" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A75" s="6" t="s">
+      <c r="B77" t="s">
+        <v>109</v>
+      </c>
+      <c r="C77" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
         <v>55</v>
       </c>
-      <c r="B75" t="s">
-        <v>109</v>
-      </c>
-      <c r="C75" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" s="6" t="s">
+      <c r="B78" t="s">
+        <v>109</v>
+      </c>
+      <c r="C78" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
         <v>59</v>
       </c>
-      <c r="B76" t="s">
-        <v>109</v>
-      </c>
-      <c r="C76" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" s="6" t="s">
+      <c r="B79" t="s">
+        <v>109</v>
+      </c>
+      <c r="C79" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
         <v>60</v>
       </c>
-      <c r="B77" t="s">
-        <v>109</v>
-      </c>
-      <c r="C77" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" s="8" t="s">
+      <c r="B80" t="s">
+        <v>109</v>
+      </c>
+      <c r="C80" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B78" t="s">
-        <v>109</v>
-      </c>
-      <c r="C78" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A79" s="9" t="s">
+      <c r="B81" t="s">
+        <v>109</v>
+      </c>
+      <c r="C81" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B79" t="s">
-        <v>109</v>
-      </c>
-      <c r="C79" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A80" s="6" t="s">
+      <c r="B82" t="s">
+        <v>109</v>
+      </c>
+      <c r="C82" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
         <v>56</v>
       </c>
-      <c r="B80" t="s">
-        <v>109</v>
-      </c>
-      <c r="C80" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A81" s="6" t="s">
+      <c r="B83" t="s">
+        <v>109</v>
+      </c>
+      <c r="C83" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
         <v>85</v>
       </c>
-      <c r="B81" t="s">
-        <v>109</v>
-      </c>
-      <c r="C81" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A82" s="6" t="s">
+      <c r="B84" t="s">
+        <v>109</v>
+      </c>
+      <c r="C84" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
         <v>71</v>
       </c>
-      <c r="B82" t="s">
-        <v>109</v>
-      </c>
-      <c r="C82" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A83" s="6" t="s">
+      <c r="B85" t="s">
+        <v>109</v>
+      </c>
+      <c r="C85" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
         <v>70</v>
       </c>
-      <c r="B83" t="s">
-        <v>109</v>
-      </c>
-      <c r="C83" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A84" s="6" t="s">
+      <c r="B86" t="s">
+        <v>109</v>
+      </c>
+      <c r="C86" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
         <v>118</v>
-      </c>
-      <c r="B84" t="s">
-        <v>109</v>
-      </c>
-      <c r="C84" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A85" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="B85" t="s">
-        <v>109</v>
-      </c>
-      <c r="C85" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="B86" t="s">
-        <v>109</v>
-      </c>
-      <c r="C86" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A87" s="6" t="s">
-        <v>121</v>
       </c>
       <c r="B87" t="s">
         <v>109</v>
@@ -3229,8 +3285,8 @@
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A88" s="6" t="s">
-        <v>122</v>
+      <c r="A88" t="s">
+        <v>119</v>
       </c>
       <c r="B88" t="s">
         <v>109</v>
@@ -3240,8 +3296,8 @@
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A89" s="6" t="s">
-        <v>123</v>
+      <c r="A89" t="s">
+        <v>120</v>
       </c>
       <c r="B89" t="s">
         <v>109</v>
@@ -3251,337 +3307,370 @@
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A90" s="6" t="s">
+      <c r="A90" t="s">
+        <v>121</v>
+      </c>
+      <c r="B90" t="s">
+        <v>109</v>
+      </c>
+      <c r="C90" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>122</v>
+      </c>
+      <c r="B91" t="s">
+        <v>109</v>
+      </c>
+      <c r="C91" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>123</v>
+      </c>
+      <c r="B92" t="s">
+        <v>109</v>
+      </c>
+      <c r="C92" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
         <v>35</v>
       </c>
-      <c r="B90" t="s">
-        <v>109</v>
-      </c>
-      <c r="C90" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A91" s="6" t="s">
+      <c r="B93" t="s">
+        <v>109</v>
+      </c>
+      <c r="C93" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
         <v>36</v>
       </c>
-      <c r="B91" t="s">
-        <v>109</v>
-      </c>
-      <c r="C91" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A92" s="6" t="s">
+      <c r="B94" t="s">
+        <v>109</v>
+      </c>
+      <c r="C94" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
         <v>45</v>
       </c>
-      <c r="B92" t="s">
-        <v>109</v>
-      </c>
-      <c r="C92" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A93" s="6" t="s">
+      <c r="B95" t="s">
+        <v>109</v>
+      </c>
+      <c r="C95" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
         <v>46</v>
       </c>
-      <c r="B93" t="s">
-        <v>109</v>
-      </c>
-      <c r="C93" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A94" s="6" t="s">
+      <c r="B96" t="s">
+        <v>109</v>
+      </c>
+      <c r="C96" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
         <v>47</v>
       </c>
-      <c r="B94" t="s">
-        <v>109</v>
-      </c>
-      <c r="C94" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A95" s="6" t="s">
+      <c r="B97" t="s">
+        <v>109</v>
+      </c>
+      <c r="C97" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
         <v>48</v>
       </c>
-      <c r="B95" t="s">
-        <v>109</v>
-      </c>
-      <c r="C95" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A96" s="6" t="s">
+      <c r="B98" t="s">
+        <v>109</v>
+      </c>
+      <c r="C98" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
         <v>44</v>
       </c>
-      <c r="B96" t="s">
-        <v>109</v>
-      </c>
-      <c r="C96" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A97" s="6" t="s">
+      <c r="B99" t="s">
+        <v>109</v>
+      </c>
+      <c r="C99" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
         <v>37</v>
       </c>
-      <c r="B97" t="s">
-        <v>109</v>
-      </c>
-      <c r="C97" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A98" s="6" t="s">
+      <c r="B100" t="s">
+        <v>109</v>
+      </c>
+      <c r="C100" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
         <v>43</v>
       </c>
-      <c r="B98" t="s">
-        <v>109</v>
-      </c>
-      <c r="C98" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A99" s="6" t="s">
+      <c r="B101" t="s">
+        <v>109</v>
+      </c>
+      <c r="C101" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
         <v>38</v>
       </c>
-      <c r="B99" t="s">
-        <v>109</v>
-      </c>
-      <c r="C99" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A100" s="6" t="s">
+      <c r="B102" t="s">
+        <v>109</v>
+      </c>
+      <c r="C102" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
         <v>28</v>
       </c>
-      <c r="B100" t="s">
-        <v>109</v>
-      </c>
-      <c r="C100" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A101" s="6" t="s">
+      <c r="B103" t="s">
+        <v>109</v>
+      </c>
+      <c r="C103" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
         <v>29</v>
       </c>
-      <c r="B101" t="s">
-        <v>109</v>
-      </c>
-      <c r="C101" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A102" s="6" t="s">
+      <c r="B104" t="s">
+        <v>109</v>
+      </c>
+      <c r="C104" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
         <v>30</v>
       </c>
-      <c r="B102" t="s">
-        <v>109</v>
-      </c>
-      <c r="C102" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A103" s="6" t="s">
+      <c r="B105" t="s">
+        <v>109</v>
+      </c>
+      <c r="C105" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
         <v>31</v>
       </c>
-      <c r="B103" t="s">
-        <v>109</v>
-      </c>
-      <c r="C103" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A104" s="6" t="s">
+      <c r="B106" t="s">
+        <v>109</v>
+      </c>
+      <c r="C106" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
         <v>32</v>
       </c>
-      <c r="B104" t="s">
-        <v>109</v>
-      </c>
-      <c r="C104" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A105" s="6" t="s">
+      <c r="B107" t="s">
+        <v>109</v>
+      </c>
+      <c r="C107" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
         <v>33</v>
       </c>
-      <c r="B105" t="s">
-        <v>109</v>
-      </c>
-      <c r="C105" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A106" s="6" t="s">
+      <c r="B108" t="s">
+        <v>109</v>
+      </c>
+      <c r="C108" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
         <v>42</v>
       </c>
-      <c r="B106" t="s">
-        <v>109</v>
-      </c>
-      <c r="C106" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A107" s="6" t="s">
+      <c r="B109" t="s">
+        <v>109</v>
+      </c>
+      <c r="C109" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
         <v>39</v>
       </c>
-      <c r="B107" t="s">
-        <v>109</v>
-      </c>
-      <c r="C107" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A108" s="6" t="s">
+      <c r="B110" t="s">
+        <v>109</v>
+      </c>
+      <c r="C110" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
         <v>34</v>
       </c>
-      <c r="B108" t="s">
-        <v>109</v>
-      </c>
-      <c r="C108" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A109" s="6" t="s">
+      <c r="B111" t="s">
+        <v>109</v>
+      </c>
+      <c r="C111" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
         <v>41</v>
       </c>
-      <c r="B109" t="s">
-        <v>109</v>
-      </c>
-      <c r="C109" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A110" s="6" t="s">
+      <c r="B112" t="s">
+        <v>109</v>
+      </c>
+      <c r="C112" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
         <v>40</v>
       </c>
-      <c r="B110" t="s">
-        <v>109</v>
-      </c>
-      <c r="C110" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A111" s="6" t="s">
+      <c r="B113" t="s">
+        <v>109</v>
+      </c>
+      <c r="C113" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
         <v>97</v>
       </c>
-      <c r="B111" t="s">
-        <v>109</v>
-      </c>
-      <c r="C111" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A112" s="6" t="s">
+      <c r="B114" t="s">
+        <v>109</v>
+      </c>
+      <c r="C114" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
         <v>96</v>
       </c>
-      <c r="B112" t="s">
-        <v>109</v>
-      </c>
-      <c r="C112" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A113" s="6" t="s">
+      <c r="B115" t="s">
+        <v>109</v>
+      </c>
+      <c r="C115" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
         <v>95</v>
       </c>
-      <c r="B113" t="s">
-        <v>109</v>
-      </c>
-      <c r="C113" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A114" s="6" t="s">
+      <c r="B116" t="s">
+        <v>109</v>
+      </c>
+      <c r="C116" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
         <v>15</v>
       </c>
-      <c r="B114" t="s">
-        <v>109</v>
-      </c>
-      <c r="C114" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A115" s="6" t="s">
+      <c r="B117" t="s">
+        <v>109</v>
+      </c>
+      <c r="C117" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
         <v>124</v>
       </c>
-      <c r="B115" t="s">
-        <v>109</v>
-      </c>
-      <c r="C115" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A116" s="6" t="s">
+      <c r="B118" t="s">
+        <v>109</v>
+      </c>
+      <c r="C118" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
         <v>125</v>
       </c>
-      <c r="B116" t="s">
-        <v>109</v>
-      </c>
-      <c r="C116" t="s">
+      <c r="B119" t="s">
+        <v>109</v>
+      </c>
+      <c r="C119" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A117" s="6" t="s">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
         <v>3</v>
       </c>
-      <c r="B117" t="s">
-        <v>109</v>
-      </c>
-      <c r="C117" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A118" s="6" t="s">
+      <c r="B120" t="s">
+        <v>109</v>
+      </c>
+      <c r="C120" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
         <v>4</v>
       </c>
-      <c r="B118" t="s">
-        <v>109</v>
-      </c>
-      <c r="C118" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A119" s="6" t="s">
+      <c r="B121" t="s">
+        <v>109</v>
+      </c>
+      <c r="C121" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
         <v>2</v>
       </c>
-      <c r="B119" t="s">
-        <v>109</v>
-      </c>
-      <c r="C119" t="s">
+      <c r="B122" t="s">
+        <v>109</v>
+      </c>
+      <c r="C122" t="s">
         <v>110</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C119"/>
+  <autoFilter ref="A1:C122" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>